<commit_message>
UPD: End of course HTML5/CSS3 part 2
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A753E678-BB25-44D1-822A-C8D5591746C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8612B0-2CDB-4F34-8474-EC68198177C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15600" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="282">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3022,7 +3022,7 @@
   <dimension ref="A2:AZ195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT10" sqref="AT10"/>
+      <selection activeCell="AT11" sqref="AT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3799,7 +3799,9 @@
       <c r="AF10" s="210" t="s">
         <v>281</v>
       </c>
-      <c r="AG10" s="194"/>
+      <c r="AG10" s="194">
+        <v>7</v>
+      </c>
       <c r="AH10" s="194"/>
       <c r="AI10" s="194"/>
       <c r="AJ10" s="194"/>
@@ -3816,6 +3818,9 @@
       </c>
       <c r="AS10" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT10" s="209" t="s">
+        <v>279</v>
       </c>
       <c r="AX10" s="191">
         <v>0.2</v>
@@ -18336,7 +18341,9 @@
   </sheetPr>
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18385,11 +18392,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D27)</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E27)/COUNTA(B4:B27)</f>
-        <v>0.25</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F27)=0,"-",MIN(F4:F27))</f>
@@ -18401,7 +18408,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(H4:H27)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -18555,13 +18562,22 @@
       <c r="C10" s="14">
         <v>8</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="14">
+        <v>3</v>
+      </c>
       <c r="E10" s="15">
-        <v>0</v>
-      </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="42">
+        <v>43864</v>
+      </c>
+      <c r="G10" s="42">
+        <v>43864</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
@@ -22576,11 +22592,11 @@
       </c>
       <c r="D3" s="54">
         <f>SUM(D4:D7)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E3" s="55">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>7.9117063492063489E-2</v>
+        <v>0.10863095238095237</v>
       </c>
       <c r="F3" s="56">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -22592,7 +22608,7 @@
       </c>
       <c r="H3" s="54">
         <f>SUM(H4:H7)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -22605,11 +22621,11 @@
       </c>
       <c r="D4" s="58">
         <f t="shared" ref="D4:H4" si="0">D10</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E4" s="59">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
       <c r="F4" s="60">
         <f>IF(F10="-","",F10)</f>
@@ -22621,7 +22637,7 @@
       </c>
       <c r="H4" s="61">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -22634,11 +22650,11 @@
       </c>
       <c r="D5" s="63">
         <f>D29</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="64">
         <f>E29</f>
-        <v>0.1111111111111111</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F5" s="63">
         <f>IF(F29="-","",F29)</f>
@@ -22650,7 +22666,7 @@
       </c>
       <c r="H5" s="65">
         <f>H29</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -22742,11 +22758,11 @@
       </c>
       <c r="D10" s="54">
         <f>SUM(D11:D26)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10" s="55">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
       <c r="F10" s="56">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -22758,7 +22774,7 @@
       </c>
       <c r="H10" s="54">
         <f>SUM(H11:H26)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -22802,23 +22818,23 @@
       </c>
       <c r="D12" s="63">
         <f>'LE COMMENCEMENT'!D10</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="64">
         <f>'LE COMMENCEMENT'!E10</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F12" s="89">
         <f>IF('LE COMMENCEMENT'!F10="","",'LE COMMENCEMENT'!F10)</f>
-        <v/>
-      </c>
-      <c r="G12" s="89" t="str">
+        <v>43864</v>
+      </c>
+      <c r="G12" s="89">
         <f>IF('LE COMMENCEMENT'!G10="","",'LE COMMENCEMENT'!G10)</f>
-        <v/>
-      </c>
-      <c r="H12" s="65" t="str">
+        <v>43864</v>
+      </c>
+      <c r="H12" s="65">
         <f t="shared" ref="H12:H14" si="1">IF(D12=0,"",C12-D12)</f>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -23236,11 +23252,11 @@
       </c>
       <c r="D29" s="54">
         <f>SUM(D30:D47)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E29" s="55">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.1111111111111111</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F29" s="56">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -23252,7 +23268,7 @@
       </c>
       <c r="H29" s="54">
         <f>SUM(H30:H47)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -23296,23 +23312,23 @@
       </c>
       <c r="D31" s="63">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" s="64">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F31" s="89">
         <f t="shared" ref="F31:G33" si="15">IF(F12="","",F12)</f>
-        <v/>
-      </c>
-      <c r="G31" s="89" t="str">
+        <v>43864</v>
+      </c>
+      <c r="G31" s="89">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="H31" s="65" t="str">
+        <v>43864</v>
+      </c>
+      <c r="H31" s="65">
         <f>IF(D31=0,"",C31-D31)</f>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course HTML5/CSS3 part 3
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8612B0-2CDB-4F34-8474-EC68198177C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2201AAE-2D38-4650-A2F0-DED767364328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15600" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="282">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3022,7 +3022,7 @@
   <dimension ref="A2:AZ195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT11" sqref="AT11"/>
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3802,7 +3802,9 @@
       <c r="AG10" s="194">
         <v>7</v>
       </c>
-      <c r="AH10" s="194"/>
+      <c r="AH10" s="194">
+        <v>8</v>
+      </c>
       <c r="AI10" s="194"/>
       <c r="AJ10" s="194"/>
       <c r="AK10" s="194"/>
@@ -3955,6 +3957,9 @@
       </c>
       <c r="AS11" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT11" s="209" t="s">
+        <v>279</v>
       </c>
       <c r="AX11" s="191">
         <v>0.4</v>
@@ -18342,7 +18347,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -18392,11 +18397,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D27)</f>
-        <v>29</v>
+        <v>31.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E27)/COUNTA(B4:B27)</f>
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F27)=0,"-",MIN(F4:F27))</f>
@@ -18408,7 +18413,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(H4:H27)</f>
-        <v>41</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -18586,13 +18591,22 @@
       <c r="C11" s="14">
         <v>8</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="14">
+        <v>2.5</v>
+      </c>
       <c r="E11" s="15">
-        <v>0</v>
-      </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="42">
+        <v>43865</v>
+      </c>
+      <c r="G11" s="42">
+        <v>43865</v>
+      </c>
+      <c r="H11" s="16">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
@@ -22592,11 +22606,11 @@
       </c>
       <c r="D3" s="54">
         <f>SUM(D4:D7)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E3" s="55">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.10863095238095237</v>
+        <v>0.13814484126984128</v>
       </c>
       <c r="F3" s="56">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -22608,7 +22622,7 @@
       </c>
       <c r="H3" s="54">
         <f>SUM(H4:H7)</f>
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -22621,11 +22635,11 @@
       </c>
       <c r="D4" s="58">
         <f t="shared" ref="D4:H4" si="0">D10</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="E4" s="59">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
       <c r="F4" s="60">
         <f>IF(F10="-","",F10)</f>
@@ -22637,7 +22651,7 @@
       </c>
       <c r="H4" s="61">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -22650,11 +22664,11 @@
       </c>
       <c r="D5" s="63">
         <f>D29</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="E5" s="64">
         <f>E29</f>
-        <v>0.16666666666666666</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F5" s="63">
         <f>IF(F29="-","",F29)</f>
@@ -22666,7 +22680,7 @@
       </c>
       <c r="H5" s="65">
         <f>H29</f>
-        <v>20</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -22758,11 +22772,11 @@
       </c>
       <c r="D10" s="54">
         <f>SUM(D11:D26)</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="E10" s="55">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
       <c r="F10" s="56">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -22774,7 +22788,7 @@
       </c>
       <c r="H10" s="54">
         <f>SUM(H11:H26)</f>
-        <v>11</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -22848,23 +22862,23 @@
       </c>
       <c r="D13" s="63">
         <f>'LE COMMENCEMENT'!D11</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E13" s="64">
         <f>'LE COMMENCEMENT'!E11</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F13" s="89">
         <f>IF('LE COMMENCEMENT'!F11="","",'LE COMMENCEMENT'!F11)</f>
-        <v/>
-      </c>
-      <c r="G13" s="89" t="str">
+        <v>43865</v>
+      </c>
+      <c r="G13" s="89">
         <f>IF('LE COMMENCEMENT'!G11="","",'LE COMMENCEMENT'!G11)</f>
-        <v/>
-      </c>
-      <c r="H13" s="65" t="str">
+        <v>43865</v>
+      </c>
+      <c r="H13" s="65">
         <f t="shared" si="1"/>
-        <v/>
+        <v>5.5</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -23252,11 +23266,11 @@
       </c>
       <c r="D29" s="54">
         <f>SUM(D30:D47)</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="E29" s="55">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.16666666666666666</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F29" s="56">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -23268,7 +23282,7 @@
       </c>
       <c r="H29" s="54">
         <f>SUM(H30:H47)</f>
-        <v>20</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -23342,23 +23356,23 @@
       </c>
       <c r="D32" s="63">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E32" s="64">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F32" s="89">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="G32" s="89" t="str">
+        <v>43865</v>
+      </c>
+      <c r="G32" s="89">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="H32" s="65" t="str">
+        <v>43865</v>
+      </c>
+      <c r="H32" s="65">
         <f t="shared" ref="H32:H47" si="16">IF(D32=0,"",C32-D32)</f>
-        <v/>
+        <v>5.5</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course HTML5/CSS3 part 4
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2201AAE-2D38-4650-A2F0-DED767364328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308DEE96-9088-434F-BC30-0DD0958C5577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15600" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="282">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3022,7 +3022,7 @@
   <dimension ref="A2:AZ195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+      <selection activeCell="AT13" sqref="AT13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3805,10 +3805,18 @@
       <c r="AH10" s="194">
         <v>8</v>
       </c>
-      <c r="AI10" s="194"/>
-      <c r="AJ10" s="194"/>
-      <c r="AK10" s="194"/>
-      <c r="AL10" s="197"/>
+      <c r="AI10" s="194">
+        <v>9</v>
+      </c>
+      <c r="AJ10" s="194" t="s">
+        <v>257</v>
+      </c>
+      <c r="AK10" s="194" t="s">
+        <v>257</v>
+      </c>
+      <c r="AL10" s="197" t="s">
+        <v>257</v>
+      </c>
       <c r="AP10" s="13" t="s">
         <v>144</v>
       </c>
@@ -4044,7 +4052,9 @@
       <c r="AD12" s="197">
         <v>10</v>
       </c>
-      <c r="AF12" s="197"/>
+      <c r="AF12" s="197" t="s">
+        <v>257</v>
+      </c>
       <c r="AG12" s="194"/>
       <c r="AH12" s="194"/>
       <c r="AI12" s="194"/>
@@ -4062,6 +4072,9 @@
       </c>
       <c r="AS12" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT12" s="209" t="s">
+        <v>279</v>
       </c>
       <c r="AX12" s="191">
         <v>0.5</v>
@@ -18347,7 +18360,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -18397,11 +18410,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D27)</f>
-        <v>31.5</v>
+        <v>34.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E27)/COUNTA(B4:B27)</f>
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F27)=0,"-",MIN(F4:F27))</f>
@@ -18413,7 +18426,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(H4:H27)</f>
-        <v>46.5</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -18615,13 +18628,22 @@
       <c r="C12" s="14">
         <v>8</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="14">
+        <v>3</v>
+      </c>
       <c r="E12" s="15">
-        <v>0</v>
-      </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="42">
+        <v>43866</v>
+      </c>
+      <c r="G12" s="42">
+        <v>43866</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
@@ -22606,11 +22628,11 @@
       </c>
       <c r="D3" s="54">
         <f>SUM(D4:D7)</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E3" s="55">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.13814484126984128</v>
+        <v>0.16765873015873017</v>
       </c>
       <c r="F3" s="56">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -22622,7 +22644,7 @@
       </c>
       <c r="H3" s="54">
         <f>SUM(H4:H7)</f>
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -22635,11 +22657,11 @@
       </c>
       <c r="D4" s="58">
         <f t="shared" ref="D4:H4" si="0">D10</f>
-        <v>7.5</v>
+        <v>10.5</v>
       </c>
       <c r="E4" s="59">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="F4" s="60">
         <f>IF(F10="-","",F10)</f>
@@ -22651,7 +22673,7 @@
       </c>
       <c r="H4" s="61">
         <f t="shared" si="0"/>
-        <v>16.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -22664,11 +22686,11 @@
       </c>
       <c r="D5" s="63">
         <f>D29</f>
-        <v>12.5</v>
+        <v>15.5</v>
       </c>
       <c r="E5" s="64">
         <f>E29</f>
-        <v>0.22222222222222221</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="F5" s="63">
         <f>IF(F29="-","",F29)</f>
@@ -22680,7 +22702,7 @@
       </c>
       <c r="H5" s="65">
         <f>H29</f>
-        <v>25.5</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -22772,11 +22794,11 @@
       </c>
       <c r="D10" s="54">
         <f>SUM(D11:D26)</f>
-        <v>7.5</v>
+        <v>10.5</v>
       </c>
       <c r="E10" s="55">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="F10" s="56">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -22788,7 +22810,7 @@
       </c>
       <c r="H10" s="54">
         <f>SUM(H11:H26)</f>
-        <v>16.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -22892,23 +22914,23 @@
       </c>
       <c r="D14" s="63">
         <f>'LE COMMENCEMENT'!D12</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" s="64">
         <f>'LE COMMENCEMENT'!E12</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F14" s="89">
         <f>IF('LE COMMENCEMENT'!F12="","",'LE COMMENCEMENT'!F12)</f>
-        <v/>
-      </c>
-      <c r="G14" s="89" t="str">
+        <v>43866</v>
+      </c>
+      <c r="G14" s="89">
         <f>IF('LE COMMENCEMENT'!G12="","",'LE COMMENCEMENT'!G12)</f>
-        <v/>
-      </c>
-      <c r="H14" s="65" t="str">
+        <v>43866</v>
+      </c>
+      <c r="H14" s="65">
         <f t="shared" si="1"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -23266,11 +23288,11 @@
       </c>
       <c r="D29" s="54">
         <f>SUM(D30:D47)</f>
-        <v>12.5</v>
+        <v>15.5</v>
       </c>
       <c r="E29" s="55">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.22222222222222221</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="F29" s="56">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -23282,7 +23304,7 @@
       </c>
       <c r="H29" s="54">
         <f>SUM(H30:H47)</f>
-        <v>25.5</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -23386,23 +23408,23 @@
       </c>
       <c r="D33" s="63">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" s="64">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F33" s="89">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="G33" s="89" t="str">
+        <v>43866</v>
+      </c>
+      <c r="G33" s="89">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="H33" s="65" t="str">
+        <v>43866</v>
+      </c>
+      <c r="H33" s="65">
         <f t="shared" si="16"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course JavaScript Introduction
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308DEE96-9088-434F-BC30-0DD0958C5577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E6B2DC-04DB-4E3E-BF23-F24EC5C08A82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15600" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="282">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3022,7 +3022,7 @@
   <dimension ref="A2:AZ195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT13" sqref="AT13"/>
+      <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4055,12 +4055,24 @@
       <c r="AF12" s="197" t="s">
         <v>257</v>
       </c>
-      <c r="AG12" s="194"/>
-      <c r="AH12" s="194"/>
-      <c r="AI12" s="194"/>
-      <c r="AJ12" s="194"/>
-      <c r="AK12" s="194"/>
-      <c r="AL12" s="197"/>
+      <c r="AG12" s="194" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH12" s="194" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI12" s="194">
+        <v>10</v>
+      </c>
+      <c r="AJ12" s="194">
+        <v>10</v>
+      </c>
+      <c r="AK12" s="194" t="s">
+        <v>257</v>
+      </c>
+      <c r="AL12" s="197" t="s">
+        <v>257</v>
+      </c>
       <c r="AP12" s="13" t="s">
         <v>146</v>
       </c>
@@ -4215,6 +4227,9 @@
       </c>
       <c r="AS13" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT13" s="209" t="s">
+        <v>279</v>
       </c>
       <c r="AX13" s="191">
         <v>0.6</v>
@@ -4296,24 +4311,26 @@
       <c r="AD14" s="197" t="s">
         <v>257</v>
       </c>
-      <c r="AF14" s="197"/>
+      <c r="AF14" s="197">
+        <v>10</v>
+      </c>
       <c r="AG14" s="194"/>
       <c r="AH14" s="194"/>
       <c r="AI14" s="194"/>
       <c r="AJ14" s="194"/>
       <c r="AK14" s="194"/>
       <c r="AL14" s="197"/>
-      <c r="AP14" s="13" t="s">
+      <c r="AP14" s="158" t="s">
+        <v>156</v>
+      </c>
+      <c r="AQ14" s="170">
         <v>6</v>
       </c>
-      <c r="AQ14" s="14">
-        <v>12</v>
-      </c>
       <c r="AR14" s="176">
-        <v>11</v>
-      </c>
-      <c r="AS14" s="4" t="s">
-        <v>0</v>
+        <v>113</v>
+      </c>
+      <c r="AS14" s="157" t="s">
+        <v>141</v>
       </c>
       <c r="AX14" s="191">
         <v>0.8</v>
@@ -4437,16 +4454,16 @@
         <f t="shared" ref="AL15" si="48">AK15+1</f>
         <v>43890</v>
       </c>
-      <c r="AP15" s="158" t="s">
-        <v>156</v>
-      </c>
-      <c r="AQ15" s="170">
+      <c r="AP15" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="AQ15" s="76">
         <v>6</v>
       </c>
       <c r="AR15" s="176">
-        <v>113</v>
-      </c>
-      <c r="AS15" s="157" t="s">
+        <v>114</v>
+      </c>
+      <c r="AS15" s="54" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4533,13 +4550,13 @@
       <c r="AK16" s="194"/>
       <c r="AL16" s="197"/>
       <c r="AP16" s="75" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AQ16" s="76">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AR16" s="176">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AS16" s="54" t="s">
         <v>141</v>
@@ -4666,13 +4683,13 @@
         <v>43897</v>
       </c>
       <c r="AP17" s="75" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="AQ17" s="76">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AR17" s="176">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AS17" s="54" t="s">
         <v>141</v>
@@ -4767,13 +4784,13 @@
       <c r="AK18" s="194"/>
       <c r="AL18" s="197"/>
       <c r="AP18" s="75" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AQ18" s="76">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AR18" s="176">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AS18" s="54" t="s">
         <v>141</v>
@@ -4898,13 +4915,13 @@
         <v>43904</v>
       </c>
       <c r="AP19" s="75" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="AQ19" s="76">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AR19" s="176">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AS19" s="54" t="s">
         <v>141</v>
@@ -4998,14 +5015,14 @@
       <c r="AJ20" s="194"/>
       <c r="AK20" s="194"/>
       <c r="AL20" s="197"/>
-      <c r="AP20" s="75" t="s">
-        <v>159</v>
+      <c r="AP20" s="80" t="s">
+        <v>152</v>
       </c>
       <c r="AQ20" s="76">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AR20" s="176">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AS20" s="54" t="s">
         <v>141</v>
@@ -5131,14 +5148,14 @@
         <f t="shared" ref="AL21" si="79">AK21+1</f>
         <v>43911</v>
       </c>
-      <c r="AP21" s="80" t="s">
-        <v>152</v>
+      <c r="AP21" s="75" t="s">
+        <v>160</v>
       </c>
       <c r="AQ21" s="76">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AR21" s="176">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AS21" s="54" t="s">
         <v>141</v>
@@ -5230,13 +5247,13 @@
       <c r="AK22" s="194"/>
       <c r="AL22" s="197"/>
       <c r="AP22" s="75" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AQ22" s="76">
         <v>8</v>
       </c>
       <c r="AR22" s="176">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AS22" s="54" t="s">
         <v>141</v>
@@ -5360,13 +5377,13 @@
         <v>43918</v>
       </c>
       <c r="AP23" s="75" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="AQ23" s="76">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="AR23" s="176">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AS23" s="54" t="s">
         <v>141</v>
@@ -5457,14 +5474,14 @@
       <c r="AJ24" s="194"/>
       <c r="AK24" s="194"/>
       <c r="AL24" s="197"/>
-      <c r="AP24" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ24" s="76">
+      <c r="AP24" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ24" s="81">
         <v>20</v>
       </c>
       <c r="AR24" s="176">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AS24" s="54" t="s">
         <v>141</v>
@@ -5587,17 +5604,17 @@
         <f t="shared" ref="AL25" si="100">AK25+1</f>
         <v>43925</v>
       </c>
-      <c r="AP25" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ25" s="81">
-        <v>20</v>
+      <c r="AP25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ25" s="14">
+        <v>8</v>
       </c>
       <c r="AR25" s="176">
-        <v>123</v>
-      </c>
-      <c r="AS25" s="54" t="s">
-        <v>141</v>
+        <v>12</v>
+      </c>
+      <c r="AS25" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5683,13 +5700,13 @@
       <c r="AK26" s="194"/>
       <c r="AL26" s="197"/>
       <c r="AP26" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AQ26" s="14">
         <v>8</v>
       </c>
       <c r="AR26" s="176">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AS26" s="4" t="s">
         <v>0</v>
@@ -5813,13 +5830,13 @@
         <v>43932</v>
       </c>
       <c r="AP27" s="13" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="AQ27" s="14">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AR27" s="176">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AS27" s="4" t="s">
         <v>0</v>
@@ -5912,13 +5929,13 @@
       <c r="AK28" s="194"/>
       <c r="AL28" s="197"/>
       <c r="AP28" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AQ28" s="14">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AR28" s="176">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AS28" s="4" t="s">
         <v>0</v>
@@ -6045,17 +6062,17 @@
         <f t="shared" ref="AL29" si="120">AK29+1</f>
         <v>43939</v>
       </c>
-      <c r="AP29" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ29" s="14">
+      <c r="AP29" s="153" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ29" s="169">
         <v>12</v>
       </c>
       <c r="AR29" s="176">
-        <v>15</v>
-      </c>
-      <c r="AS29" s="4" t="s">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="AS29" s="154" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -6144,16 +6161,16 @@
       <c r="AJ30" s="194"/>
       <c r="AK30" s="194"/>
       <c r="AL30" s="197"/>
-      <c r="AP30" s="153" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ30" s="169">
+      <c r="AP30" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ30" s="30">
         <v>12</v>
       </c>
       <c r="AR30" s="176">
-        <v>35</v>
-      </c>
-      <c r="AS30" s="154" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS30" s="21" t="s">
         <v>135</v>
       </c>
       <c r="AZ30" s="206" t="s">
@@ -6272,13 +6289,13 @@
         <v>43946</v>
       </c>
       <c r="AP31" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AQ31" s="30">
         <v>12</v>
       </c>
       <c r="AR31" s="176">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AS31" s="21" t="s">
         <v>135</v>
@@ -6367,13 +6384,13 @@
       <c r="AK32" s="194"/>
       <c r="AL32" s="197"/>
       <c r="AP32" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AQ32" s="30">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="AR32" s="176">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AS32" s="21" t="s">
         <v>135</v>
@@ -6497,13 +6514,13 @@
         <v>43953</v>
       </c>
       <c r="AP33" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AQ33" s="30">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="AR33" s="176">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AS33" s="21" t="s">
         <v>135</v>
@@ -6594,17 +6611,17 @@
       <c r="AJ34" s="194"/>
       <c r="AK34" s="194"/>
       <c r="AL34" s="197"/>
-      <c r="AP34" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ34" s="30">
+      <c r="AP34" s="13" t="s">
         <v>6</v>
       </c>
+      <c r="AQ34" s="14">
+        <v>12</v>
+      </c>
       <c r="AR34" s="176">
-        <v>39</v>
-      </c>
-      <c r="AS34" s="21" t="s">
-        <v>135</v>
+        <v>11</v>
+      </c>
+      <c r="AS34" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18359,9 +18376,7 @@
   </sheetPr>
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18410,11 +18425,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D27)</f>
-        <v>34.5</v>
+        <v>44.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E27)/COUNTA(B4:B27)</f>
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F27)=0,"-",MIN(F4:F27))</f>
@@ -18426,7 +18441,7 @@
       </c>
       <c r="H3" s="4">
         <f>SUM(H4:H27)</f>
-        <v>51.5</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -18652,13 +18667,22 @@
       <c r="C13" s="14">
         <v>20</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="14">
+        <v>10</v>
+      </c>
       <c r="E13" s="15">
-        <v>0</v>
-      </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="42">
+        <v>43873</v>
+      </c>
+      <c r="G13" s="42">
+        <v>43877</v>
+      </c>
+      <c r="H13" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
@@ -22628,11 +22652,11 @@
       </c>
       <c r="D3" s="54">
         <f>SUM(D4:D7)</f>
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E3" s="55">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.16765873015873017</v>
+        <v>0.23288690476190474</v>
       </c>
       <c r="F3" s="56">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -22644,7 +22668,7 @@
       </c>
       <c r="H3" s="54">
         <f>SUM(H4:H7)</f>
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -22657,11 +22681,11 @@
       </c>
       <c r="D4" s="58">
         <f t="shared" ref="D4:H4" si="0">D10</f>
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
       <c r="E4" s="59">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.3125</v>
       </c>
       <c r="F4" s="60">
         <f>IF(F10="-","",F10)</f>
@@ -22673,7 +22697,7 @@
       </c>
       <c r="H4" s="61">
         <f t="shared" si="0"/>
-        <v>21.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -22686,11 +22710,11 @@
       </c>
       <c r="D5" s="63">
         <f>D29</f>
-        <v>15.5</v>
+        <v>25.5</v>
       </c>
       <c r="E5" s="64">
         <f>E29</f>
-        <v>0.27777777777777779</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F5" s="63">
         <f>IF(F29="-","",F29)</f>
@@ -22702,7 +22726,7 @@
       </c>
       <c r="H5" s="65">
         <f>H29</f>
-        <v>30.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -22715,11 +22739,11 @@
       </c>
       <c r="D6" s="63">
         <f>D50</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E6" s="64">
         <f>E50</f>
-        <v>0.14285714285714285</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="F6" s="63">
         <f>IF(F50="-","",F50)</f>
@@ -22731,7 +22755,7 @@
       </c>
       <c r="H6" s="65">
         <f>H50</f>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -22794,11 +22818,11 @@
       </c>
       <c r="D10" s="54">
         <f>SUM(D11:D26)</f>
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
       <c r="E10" s="55">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>0.25</v>
+        <v>0.3125</v>
       </c>
       <c r="F10" s="56">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -22810,7 +22834,7 @@
       </c>
       <c r="H10" s="54">
         <f>SUM(H11:H26)</f>
-        <v>21.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -22944,23 +22968,23 @@
       </c>
       <c r="D15" s="63">
         <f>'LE COMMENCEMENT'!D13</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E15" s="64">
         <f>'LE COMMENCEMENT'!E13</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F15" s="89">
         <f>IF('LE COMMENCEMENT'!F13="","",'LE COMMENCEMENT'!F13)</f>
-        <v/>
-      </c>
-      <c r="G15" s="89" t="str">
+        <v>43873</v>
+      </c>
+      <c r="G15" s="89">
         <f>IF('LE COMMENCEMENT'!G13="","",'LE COMMENCEMENT'!G13)</f>
-        <v/>
-      </c>
-      <c r="H15" s="65" t="str">
+        <v>43877</v>
+      </c>
+      <c r="H15" s="65">
         <f t="shared" ref="H15" si="2">IF(D15=0,"",C15-D15)</f>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -23288,11 +23312,11 @@
       </c>
       <c r="D29" s="54">
         <f>SUM(D30:D47)</f>
-        <v>15.5</v>
+        <v>25.5</v>
       </c>
       <c r="E29" s="55">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.27777777777777779</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F29" s="56">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -23304,7 +23328,7 @@
       </c>
       <c r="H29" s="54">
         <f>SUM(H30:H47)</f>
-        <v>30.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -23492,23 +23516,23 @@
       </c>
       <c r="D37" s="63">
         <f>D15</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E37" s="64">
         <f>E15</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F37" s="89">
         <f>IF(F15="","",F15)</f>
-        <v/>
-      </c>
-      <c r="G37" s="89" t="str">
+        <v>43873</v>
+      </c>
+      <c r="G37" s="89">
         <f>IF(G15="","",G15)</f>
-        <v/>
-      </c>
-      <c r="H37" s="65" t="str">
+        <v>43877</v>
+      </c>
+      <c r="H37" s="65">
         <f t="shared" si="16"/>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -23734,11 +23758,11 @@
       </c>
       <c r="D50" s="54">
         <f>SUM(D51:D57)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E50" s="55">
         <f>SUM(E51:E57)/COUNTA(B51:B57)</f>
-        <v>0.14285714285714285</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="F50" s="56">
         <f>IF(MIN(F51:F57)=0,"-",MIN(F51:F57))</f>
@@ -23750,7 +23774,7 @@
       </c>
       <c r="H50" s="54">
         <f>SUM(H51:H57)</f>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -23795,23 +23819,23 @@
       </c>
       <c r="D52" s="63">
         <f>D15</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E52" s="64">
         <f>E15</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="89" t="str">
+        <v>1</v>
+      </c>
+      <c r="F52" s="89">
         <f>IF(F15="","",F15)</f>
-        <v/>
-      </c>
-      <c r="G52" s="89" t="str">
+        <v>43873</v>
+      </c>
+      <c r="G52" s="89">
         <f>IF(G15="","",G15)</f>
-        <v/>
-      </c>
-      <c r="H52" s="65" t="str">
+        <v>43877</v>
+      </c>
+      <c r="H52" s="65">
         <f t="shared" ref="H52:H57" si="17">IF(D52=0,"",C52-D52)</f>
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Web Accessibility part 1
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC8C4A5-01BD-45A9-B344-79B0B0C95633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A2FEF4-AD96-4FBD-9C9D-9903F8A1C3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3061,7 +3061,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT16" sqref="AT16"/>
+      <selection activeCell="AT17" sqref="AT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4369,9 +4369,15 @@
       <c r="AI14" s="166" t="s">
         <v>255</v>
       </c>
-      <c r="AJ14" s="166"/>
-      <c r="AK14" s="166"/>
-      <c r="AL14" s="169"/>
+      <c r="AJ14" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK14" s="166">
+        <v>37</v>
+      </c>
+      <c r="AL14" s="169">
+        <v>37</v>
+      </c>
       <c r="AP14" s="12" t="s">
         <v>280</v>
       </c>
@@ -4618,6 +4624,9 @@
       </c>
       <c r="AS16" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT16" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AX16" s="176" t="s">
         <v>256</v>
@@ -19537,8 +19546,8 @@
   </sheetPr>
   <dimension ref="B2:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19584,11 +19593,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>63.5</v>
+        <v>69.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.24677579365079363</v>
+        <v>0.26066468253968256</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19642,11 +19651,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -20244,11 +20253,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.3888888888888889</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20260,7 +20269,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.63052721088435371</v>
+        <v>0.55171130952380953</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20414,15 +20423,21 @@
       <c r="C35" s="63">
         <v>6</v>
       </c>
-      <c r="D35" s="63"/>
+      <c r="D35" s="63">
+        <v>6</v>
+      </c>
       <c r="E35" s="64">
-        <v>0</v>
-      </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F35" s="65">
+        <v>43882</v>
+      </c>
+      <c r="G35" s="65">
+        <v>43883</v>
+      </c>
+      <c r="H35" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Web Accessibility part 2 and Web Accessibility formation
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A2FEF4-AD96-4FBD-9C9D-9903F8A1C3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582887AD-32A6-4FAF-9D9D-CB6D1C089366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3061,7 +3061,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT17" sqref="AT17"/>
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4605,8 +4605,12 @@
       <c r="AD16" s="169">
         <v>40</v>
       </c>
-      <c r="AF16" s="169"/>
-      <c r="AG16" s="166"/>
+      <c r="AF16" s="169" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG16" s="166">
+        <v>38</v>
+      </c>
       <c r="AH16" s="166"/>
       <c r="AI16" s="166"/>
       <c r="AJ16" s="166"/>
@@ -4761,6 +4765,9 @@
       </c>
       <c r="AS17" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT17" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AX17" s="164" t="s">
         <v>257</v>
@@ -19547,7 +19554,7 @@
   <dimension ref="B2:I68"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19593,11 +19600,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>69.5</v>
+        <v>74.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.26066468253968256</v>
+        <v>0.2745535714285714</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19651,11 +19658,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -20253,11 +20260,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20269,7 +20276,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.55171130952380953</v>
+        <v>0.46263227513227512</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20447,15 +20454,21 @@
       <c r="C36" s="63">
         <v>4</v>
       </c>
-      <c r="D36" s="63"/>
+      <c r="D36" s="63">
+        <v>5</v>
+      </c>
       <c r="E36" s="64">
-        <v>0</v>
-      </c>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F36" s="65">
+        <v>43885</v>
+      </c>
+      <c r="G36" s="65">
+        <v>43885</v>
+      </c>
+      <c r="H36" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Sass and Compass
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582887AD-32A6-4FAF-9D9D-CB6D1C089366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64FBC9D-732C-4358-A068-C418DE59CDB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3061,7 +3061,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH16" sqref="AH16"/>
+      <selection activeCell="AT19" sqref="AT19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4611,10 +4611,18 @@
       <c r="AG16" s="166">
         <v>38</v>
       </c>
-      <c r="AH16" s="166"/>
-      <c r="AI16" s="166"/>
-      <c r="AJ16" s="166"/>
-      <c r="AK16" s="166"/>
+      <c r="AH16" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AI16" s="166">
+        <v>39</v>
+      </c>
+      <c r="AJ16" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK16" s="166">
+        <v>39</v>
+      </c>
       <c r="AL16" s="169"/>
       <c r="AP16" s="62" t="s">
         <v>156</v>
@@ -4870,6 +4878,9 @@
       </c>
       <c r="AS18" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT18" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AX18" s="164" t="s">
         <v>258</v>
@@ -19554,7 +19565,7 @@
   <dimension ref="B2:I68"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19600,11 +19611,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>74.5</v>
+        <v>84.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.2745535714285714</v>
+        <v>0.30406746031746035</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19629,11 +19640,11 @@
       </c>
       <c r="D4" s="49">
         <f t="shared" ref="D4:E4" si="0">D10</f>
-        <v>20.5</v>
+        <v>25.5</v>
       </c>
       <c r="E4" s="50">
         <f t="shared" si="0"/>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="F4" s="51">
         <f>IF(F10="-","",F10)</f>
@@ -19658,11 +19669,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -19766,11 +19777,11 @@
       </c>
       <c r="D10" s="45">
         <f>SUM(D11:D26)</f>
-        <v>20.5</v>
+        <v>25.5</v>
       </c>
       <c r="E10" s="46">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="F10" s="47">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -19782,7 +19793,7 @@
       </c>
       <c r="H10" s="187">
         <f>AVERAGE(H11:H26)</f>
-        <v>0.63749999999999996</v>
+        <v>0.59375</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -19982,23 +19993,23 @@
       </c>
       <c r="D18" s="53">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18" s="54">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="74" t="str">
+        <v>1</v>
+      </c>
+      <c r="F18" s="74">
         <f>IF(F38="","",F38)</f>
-        <v/>
-      </c>
-      <c r="G18" s="74" t="str">
+        <v>43887</v>
+      </c>
+      <c r="G18" s="74">
         <f>IF(G38="","",G38)</f>
-        <v/>
-      </c>
-      <c r="H18" s="189" t="str">
+        <v>43889</v>
+      </c>
+      <c r="H18" s="189">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -20260,11 +20271,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20276,7 +20287,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.46263227513227512</v>
+        <v>0.45386904761904762</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20508,15 +20519,21 @@
       <c r="C38" s="63">
         <v>8</v>
       </c>
-      <c r="D38" s="63"/>
+      <c r="D38" s="63">
+        <v>5</v>
+      </c>
       <c r="E38" s="64">
-        <v>0</v>
-      </c>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F38" s="65">
+        <v>43887</v>
+      </c>
+      <c r="G38" s="65">
+        <v>43889</v>
+      </c>
+      <c r="H38" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Flexbox
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64FBC9D-732C-4358-A068-C418DE59CDB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187301C1-74E1-4174-A46C-330372E50BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" activeTab="3" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3060,8 +3060,8 @@
   </sheetPr>
   <dimension ref="A2:AZ196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT19" sqref="AT19"/>
+    <sheetView topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4623,7 +4623,9 @@
       <c r="AK16" s="166">
         <v>39</v>
       </c>
-      <c r="AL16" s="169"/>
+      <c r="AL16" s="169" t="s">
+        <v>255</v>
+      </c>
       <c r="AP16" s="62" t="s">
         <v>156</v>
       </c>
@@ -4859,7 +4861,9 @@
       <c r="AD18" s="169">
         <v>44</v>
       </c>
-      <c r="AF18" s="169"/>
+      <c r="AF18" s="169">
+        <v>40</v>
+      </c>
       <c r="AG18" s="166"/>
       <c r="AH18" s="166"/>
       <c r="AI18" s="166"/>
@@ -5013,6 +5017,9 @@
       </c>
       <c r="AS19" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT19" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AX19" s="164" t="s">
         <v>259</v>
@@ -19564,8 +19571,8 @@
   </sheetPr>
   <dimension ref="B2:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19611,11 +19618,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>84.5</v>
+        <v>92.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.30406746031746035</v>
+        <v>0.33358134920634919</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19640,11 +19647,11 @@
       </c>
       <c r="D4" s="49">
         <f t="shared" ref="D4:E4" si="0">D10</f>
-        <v>25.5</v>
+        <v>29.5</v>
       </c>
       <c r="E4" s="50">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="F4" s="51">
         <f>IF(F10="-","",F10)</f>
@@ -19669,11 +19676,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.55555555555555558</v>
+        <v>0.61111111111111116</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -19777,11 +19784,11 @@
       </c>
       <c r="D10" s="45">
         <f>SUM(D11:D26)</f>
-        <v>25.5</v>
+        <v>29.5</v>
       </c>
       <c r="E10" s="46">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="F10" s="47">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -19793,7 +19800,7 @@
       </c>
       <c r="H10" s="187">
         <f>AVERAGE(H11:H26)</f>
-        <v>0.59375</v>
+        <v>0.58829365079365081</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -20023,23 +20030,23 @@
       </c>
       <c r="D19" s="53">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E19" s="54">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="74" t="str">
+        <v>1</v>
+      </c>
+      <c r="F19" s="74">
         <f>IF(F39="","",F39)</f>
-        <v/>
-      </c>
-      <c r="G19" s="74" t="str">
+        <v>43891</v>
+      </c>
+      <c r="G19" s="74">
         <f>IF(G39="","",G39)</f>
-        <v/>
-      </c>
-      <c r="H19" s="189" t="str">
+        <v>43891</v>
+      </c>
+      <c r="H19" s="189">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -20271,11 +20278,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.55555555555555558</v>
+        <v>0.61111111111111116</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20287,7 +20294,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.45386904761904762</v>
+        <v>0.46311327561327559</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20543,15 +20550,21 @@
       <c r="C39" s="63">
         <v>9</v>
       </c>
-      <c r="D39" s="63"/>
+      <c r="D39" s="63">
+        <v>4</v>
+      </c>
       <c r="E39" s="64">
-        <v>0</v>
-      </c>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F39" s="65">
+        <v>43891</v>
+      </c>
+      <c r="G39" s="65">
+        <v>43891</v>
+      </c>
+      <c r="H39" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course CSS Grid
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187301C1-74E1-4174-A46C-330372E50BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BCC9D6-72D9-4A4F-9E37-B0F7E686705A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" activeTab="3" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -895,7 +895,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,6 +958,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -1850,7 +1857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2495,6 +2502,9 @@
     <xf numFmtId="9" fontId="2" fillId="13" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3060,8 +3070,8 @@
   </sheetPr>
   <dimension ref="A2:AZ196"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG18" sqref="AG18"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT21" sqref="AT21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4864,9 +4874,15 @@
       <c r="AF18" s="169">
         <v>40</v>
       </c>
-      <c r="AG18" s="166"/>
-      <c r="AH18" s="166"/>
-      <c r="AI18" s="166"/>
+      <c r="AG18" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH18" s="166">
+        <v>41</v>
+      </c>
+      <c r="AI18" s="166" t="s">
+        <v>255</v>
+      </c>
       <c r="AJ18" s="166"/>
       <c r="AK18" s="166"/>
       <c r="AL18" s="169"/>
@@ -5123,6 +5139,9 @@
       <c r="AS20" s="45" t="s">
         <v>140</v>
       </c>
+      <c r="AT20" s="180" t="s">
+        <v>277</v>
+      </c>
       <c r="AX20" s="164" t="s">
         <v>260</v>
       </c>
@@ -5257,6 +5276,7 @@
       <c r="AS21" s="45" t="s">
         <v>140</v>
       </c>
+      <c r="AT21" s="216"/>
       <c r="AX21" s="164" t="s">
         <v>261</v>
       </c>
@@ -19571,8 +19591,8 @@
   </sheetPr>
   <dimension ref="B2:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19618,11 +19638,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>92.5</v>
+        <v>96.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.33358134920634919</v>
+        <v>0.34747023809523803</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19676,11 +19696,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -20278,11 +20298,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20294,7 +20314,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.46311327561327559</v>
+        <v>0.4661871693121693</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20574,15 +20594,21 @@
       <c r="C40" s="63">
         <v>8</v>
       </c>
-      <c r="D40" s="63"/>
+      <c r="D40" s="63">
+        <v>4</v>
+      </c>
       <c r="E40" s="64">
-        <v>0</v>
-      </c>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F40" s="65">
+        <v>43893</v>
+      </c>
+      <c r="G40" s="65">
+        <v>43893</v>
+      </c>
+      <c r="H40" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Responsive Web Design
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BCC9D6-72D9-4A4F-9E37-B0F7E686705A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA05948A-00E3-4B24-BC2B-02FE7306F059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -895,7 +895,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,13 +958,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -1857,7 +1850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2502,9 +2495,6 @@
     <xf numFmtId="9" fontId="2" fillId="13" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3071,7 +3061,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT21" sqref="AT21"/>
+      <selection activeCell="AT22" sqref="AT22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4883,7 +4873,9 @@
       <c r="AI18" s="166" t="s">
         <v>255</v>
       </c>
-      <c r="AJ18" s="166"/>
+      <c r="AJ18" s="166">
+        <v>42</v>
+      </c>
       <c r="AK18" s="166"/>
       <c r="AL18" s="169"/>
       <c r="AP18" s="62" t="s">
@@ -5276,7 +5268,9 @@
       <c r="AS21" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="AT21" s="216"/>
+      <c r="AT21" s="180" t="s">
+        <v>277</v>
+      </c>
       <c r="AX21" s="164" t="s">
         <v>261</v>
       </c>
@@ -19592,7 +19586,7 @@
   <dimension ref="B2:I68"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19638,11 +19632,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>96.5</v>
+        <v>104.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.34747023809523803</v>
+        <v>0.37698412698412698</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19667,11 +19661,11 @@
       </c>
       <c r="D4" s="49">
         <f t="shared" ref="D4:E4" si="0">D10</f>
-        <v>29.5</v>
+        <v>33.5</v>
       </c>
       <c r="E4" s="50">
         <f t="shared" si="0"/>
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="51">
         <f>IF(F10="-","",F10)</f>
@@ -19696,11 +19690,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -19804,11 +19798,11 @@
       </c>
       <c r="D10" s="45">
         <f>SUM(D11:D26)</f>
-        <v>29.5</v>
+        <v>33.5</v>
       </c>
       <c r="E10" s="46">
         <f>SUM(E11:E26)/COUNTA(B11:B26)</f>
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="47">
         <f>IF(MIN(F11:F26)=0,"-",MIN(F11:F26))</f>
@@ -19820,7 +19814,7 @@
       </c>
       <c r="H10" s="187">
         <f>AVERAGE(H11:H26)</f>
-        <v>0.58829365079365081</v>
+        <v>0.58975694444444438</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -20080,23 +20074,23 @@
       </c>
       <c r="D20" s="53">
         <f>D41</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E20" s="54">
         <f>E41</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="74" t="str">
+        <v>1</v>
+      </c>
+      <c r="F20" s="74">
         <f>IF(F41="","",F41)</f>
-        <v/>
-      </c>
-      <c r="G20" s="74" t="str">
+        <v>43895</v>
+      </c>
+      <c r="G20" s="74">
         <f>IF(G41="","",G41)</f>
-        <v/>
-      </c>
-      <c r="H20" s="189" t="str">
+        <v>43895</v>
+      </c>
+      <c r="H20" s="189">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -20298,11 +20292,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20314,7 +20308,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.4661871693121693</v>
+        <v>0.47648046398046395</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20618,15 +20612,21 @@
       <c r="C41" s="63">
         <v>10</v>
       </c>
-      <c r="D41" s="63"/>
+      <c r="D41" s="63">
+        <v>4</v>
+      </c>
       <c r="E41" s="64">
-        <v>0</v>
-      </c>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F41" s="65">
+        <v>43895</v>
+      </c>
+      <c r="G41" s="65">
+        <v>43895</v>
+      </c>
+      <c r="H41" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Bootstrap 4
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA05948A-00E3-4B24-BC2B-02FE7306F059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3682BD28-BA91-480F-9C11-95467F087071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="283">
   <si>
     <t>Le commencement</t>
   </si>
@@ -895,7 +895,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,6 +958,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -1850,7 +1857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2495,6 +2502,9 @@
     <xf numFmtId="9" fontId="2" fillId="13" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3061,7 +3071,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT22" sqref="AT22"/>
+      <selection activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4876,8 +4886,12 @@
       <c r="AJ18" s="166">
         <v>42</v>
       </c>
-      <c r="AK18" s="166"/>
-      <c r="AL18" s="169"/>
+      <c r="AK18" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL18" s="169">
+        <v>43</v>
+      </c>
       <c r="AP18" s="62" t="s">
         <v>149</v>
       </c>
@@ -5111,7 +5125,9 @@
       <c r="AD20" s="169">
         <v>13</v>
       </c>
-      <c r="AF20" s="169"/>
+      <c r="AF20" s="169">
+        <v>43</v>
+      </c>
       <c r="AG20" s="166"/>
       <c r="AH20" s="166"/>
       <c r="AI20" s="166"/>
@@ -5372,6 +5388,9 @@
       </c>
       <c r="AS22" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT22" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AZ22" s="179" t="s">
         <v>266</v>
@@ -19586,7 +19605,7 @@
   <dimension ref="B2:I68"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19632,11 +19651,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>104.5</v>
+        <v>108.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.37698412698412698</v>
+        <v>0.39087301587301582</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19690,11 +19709,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -20292,11 +20311,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.72222222222222221</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20308,7 +20327,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.47648046398046395</v>
+        <v>0.47816043083900223</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20636,15 +20655,21 @@
       <c r="C42" s="63">
         <v>8</v>
       </c>
-      <c r="D42" s="63"/>
+      <c r="D42" s="63">
+        <v>4</v>
+      </c>
       <c r="E42" s="64">
-        <v>0</v>
-      </c>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F42" s="65">
+        <v>43897</v>
+      </c>
+      <c r="G42" s="65">
+        <v>43898</v>
+      </c>
+      <c r="H42" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -20654,7 +20679,7 @@
       <c r="C43" s="63">
         <v>8</v>
       </c>
-      <c r="D43" s="63"/>
+      <c r="D43" s="216"/>
       <c r="E43" s="64">
         <v>0</v>
       </c>
@@ -21160,6 +21185,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>

<commit_message>
UPD: End of course CSS Architecture
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3682BD28-BA91-480F-9C11-95467F087071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7175BE40-3CBB-45AA-8DAF-36236445C0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="284">
   <si>
     <t>Le commencement</t>
   </si>
@@ -889,13 +889,16 @@
   </si>
   <si>
     <t>Tempo reduzido em</t>
+  </si>
+  <si>
+    <t>43/44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,13 +961,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -1857,7 +1853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2502,9 +2498,6 @@
     <xf numFmtId="9" fontId="2" fillId="13" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3071,7 +3064,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF20" sqref="AF20"/>
+      <selection activeCell="AT24" sqref="AT24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5125,8 +5118,8 @@
       <c r="AD20" s="169">
         <v>13</v>
       </c>
-      <c r="AF20" s="169">
-        <v>43</v>
+      <c r="AF20" s="169" t="s">
+        <v>283</v>
       </c>
       <c r="AG20" s="166"/>
       <c r="AH20" s="166"/>
@@ -5519,6 +5512,9 @@
       </c>
       <c r="AS23" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT23" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AZ23" s="179" t="s">
         <v>275</v>
@@ -19604,8 +19600,8 @@
   </sheetPr>
   <dimension ref="B2:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19651,11 +19647,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>108.5</v>
+        <v>111.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.39087301587301582</v>
+        <v>0.40476190476190477</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19709,11 +19705,11 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.77777777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -20311,11 +20307,11 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D47)</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.77777777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
@@ -20327,7 +20323,7 @@
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H47)</f>
-        <v>0.47816043083900223</v>
+        <v>0.48794973544973541</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20679,15 +20675,21 @@
       <c r="C43" s="63">
         <v>8</v>
       </c>
-      <c r="D43" s="216"/>
+      <c r="D43" s="63">
+        <v>3</v>
+      </c>
       <c r="E43" s="64">
-        <v>0</v>
-      </c>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F43" s="65">
+        <v>43898</v>
+      </c>
+      <c r="G43" s="65">
+        <v>43898</v>
+      </c>
+      <c r="H43" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.625</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Web Performance part 1
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7175BE40-3CBB-45AA-8DAF-36236445C0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF2AEF5-F86A-485E-81B1-0C2070ED629F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -3064,7 +3064,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT24" sqref="AT24"/>
+      <selection activeCell="AT25" sqref="AT25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5121,8 +5121,12 @@
       <c r="AF20" s="169" t="s">
         <v>283</v>
       </c>
-      <c r="AG20" s="166"/>
-      <c r="AH20" s="166"/>
+      <c r="AG20" s="166">
+        <v>45</v>
+      </c>
+      <c r="AH20" s="166">
+        <v>45</v>
+      </c>
       <c r="AI20" s="166"/>
       <c r="AJ20" s="166"/>
       <c r="AK20" s="166"/>
@@ -5614,6 +5618,9 @@
       </c>
       <c r="AS24" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT24" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AZ24" s="179" t="s">
         <v>267</v>
@@ -19598,10 +19605,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B2:I68"/>
+  <dimension ref="B2:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -19643,15 +19650,15 @@
       </c>
       <c r="C3" s="45">
         <f>SUM(C4:C7)</f>
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>111.5</v>
+        <v>117.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.40476190476190477</v>
+        <v>0.43172268907563027</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19701,15 +19708,15 @@
       </c>
       <c r="C5" s="53">
         <f>C29</f>
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.83333333333333337</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
@@ -19729,23 +19736,23 @@
         <v>141</v>
       </c>
       <c r="C6" s="53">
-        <f>C50</f>
+        <f>C49</f>
         <v>80</v>
       </c>
       <c r="D6" s="53">
-        <f>D50</f>
+        <f>D49</f>
         <v>15</v>
       </c>
       <c r="E6" s="54">
-        <f>E50</f>
+        <f>E49</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="F6" s="53">
-        <f>IF(F50="-","",F50)</f>
+        <f>IF(F49="-","",F49)</f>
         <v>43863</v>
       </c>
       <c r="G6" s="53" t="str">
-        <f>IF(G50="-","",G50)</f>
+        <f>IF(G49="-","",G49)</f>
         <v/>
       </c>
       <c r="H6" s="189" t="str">
@@ -19758,23 +19765,23 @@
         <v>142</v>
       </c>
       <c r="C7" s="56">
-        <f>C60</f>
+        <f>C59</f>
         <v>74</v>
       </c>
       <c r="D7" s="56">
-        <f>D60</f>
+        <f>D59</f>
         <v>0</v>
       </c>
       <c r="E7" s="57">
-        <f>E60</f>
+        <f>E59</f>
         <v>0</v>
       </c>
       <c r="F7" s="56" t="str">
-        <f>IF(F60="-","",F60)</f>
+        <f>IF(F59="-","",F59)</f>
         <v/>
       </c>
       <c r="G7" s="56" t="str">
-        <f>IF(G60="-","",G60)</f>
+        <f>IF(G59="-","",G59)</f>
         <v/>
       </c>
       <c r="H7" s="190" t="str">
@@ -20110,7 +20117,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="52" t="str">
-        <f t="shared" ref="B21:E22" si="3">B61</f>
+        <f t="shared" ref="B21:E22" si="3">B60</f>
         <v>JavaScript Avançado I</v>
       </c>
       <c r="C21" s="53">
@@ -20126,11 +20133,11 @@
         <v>0</v>
       </c>
       <c r="F21" s="74" t="str">
-        <f>IF(F61="","",F61)</f>
+        <f>IF(F60="","",F60)</f>
         <v/>
       </c>
       <c r="G21" s="74" t="str">
-        <f>IF(G61="","",G61)</f>
+        <f>IF(G60="","",G60)</f>
         <v/>
       </c>
       <c r="H21" s="189" t="str">
@@ -20156,11 +20163,11 @@
         <v>0</v>
       </c>
       <c r="F22" s="74" t="str">
-        <f>IF(F62="","",F62)</f>
+        <f>IF(F61="","",F61)</f>
         <v/>
       </c>
       <c r="G22" s="74" t="str">
-        <f>IF(G62="","",G62)</f>
+        <f>IF(G61="","",G61)</f>
         <v/>
       </c>
       <c r="H22" s="189" t="str">
@@ -20170,11 +20177,11 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="52" t="str">
-        <f>B65</f>
+        <f>B64</f>
         <v>React parte 1</v>
       </c>
       <c r="C23" s="53">
-        <f t="shared" ref="C23:E23" si="4">C65</f>
+        <f t="shared" ref="C23:E23" si="4">C64</f>
         <v>10</v>
       </c>
       <c r="D23" s="53">
@@ -20186,11 +20193,11 @@
         <v>0</v>
       </c>
       <c r="F23" s="74" t="str">
-        <f>IF(F65="","",F65)</f>
+        <f>IF(F64="","",F64)</f>
         <v/>
       </c>
       <c r="G23" s="74" t="str">
-        <f t="shared" ref="G23:G25" si="5">IF(G65="","",G65)</f>
+        <f t="shared" ref="G23:G25" si="5">IF(G64="","",G64)</f>
         <v/>
       </c>
       <c r="H23" s="189" t="str">
@@ -20200,7 +20207,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="52" t="str">
-        <f t="shared" ref="B24:E24" si="6">B66</f>
+        <f t="shared" ref="B24:E24" si="6">B65</f>
         <v>React parte 2</v>
       </c>
       <c r="C24" s="53">
@@ -20216,7 +20223,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="74" t="str">
-        <f t="shared" ref="F24" si="7">IF(F66="","",F66)</f>
+        <f t="shared" ref="F24" si="7">IF(F65="","",F65)</f>
         <v/>
       </c>
       <c r="G24" s="74" t="str">
@@ -20230,7 +20237,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="52" t="str">
-        <f t="shared" ref="B25:E25" si="8">B67</f>
+        <f t="shared" ref="B25:E25" si="8">B66</f>
         <v>React parte 3</v>
       </c>
       <c r="C25" s="53">
@@ -20246,7 +20253,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="74" t="str">
-        <f t="shared" ref="F25" si="9">IF(F67="","",F67)</f>
+        <f t="shared" ref="F25" si="9">IF(F66="","",F66)</f>
         <v/>
       </c>
       <c r="G25" s="74" t="str">
@@ -20302,28 +20309,28 @@
         <v>HTML e CSS</v>
       </c>
       <c r="C29" s="45">
-        <f>SUM(C30:C47)</f>
-        <v>188</v>
+        <f>SUM(C30:C46)</f>
+        <v>173</v>
       </c>
       <c r="D29" s="45">
-        <f>SUM(D30:D47)</f>
-        <v>63</v>
+        <f>SUM(D30:D46)</f>
+        <v>69</v>
       </c>
       <c r="E29" s="46">
-        <f>SUM(E30:E47)/COUNTA(B30:B47)</f>
-        <v>0.83333333333333337</v>
+        <f>SUM(E30:E46)/COUNTA(B30:B46)</f>
+        <v>0.94117647058823528</v>
       </c>
       <c r="F29" s="47">
-        <f>IF(MIN(F30:F47)=0,"-",MIN(F30:F47))</f>
+        <f>IF(MIN(F30:F46)=0,"-",MIN(F30:F46))</f>
         <v>43863</v>
       </c>
       <c r="G29" s="45" t="str">
-        <f>IF(COUNTBLANK(G30:G47)&lt;&gt;0,"-",MAX(G30:G47))</f>
+        <f>IF(COUNTBLANK(G30:G46)&lt;&gt;0,"-",MAX(G30:G46))</f>
         <v>-</v>
       </c>
       <c r="H29" s="187">
-        <f>AVERAGE(H30:H47)</f>
-        <v>0.48794973544973541</v>
+        <f>AVERAGE(H30:H46)</f>
+        <v>0.50120287698412691</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20352,7 +20359,7 @@
         <v>43863</v>
       </c>
       <c r="H30" s="188">
-        <f t="shared" ref="H30:H47" si="11">IF(G30="","",1-D30/C30)</f>
+        <f t="shared" ref="H30:H46" si="11">IF(G30="","",1-D30/C30)</f>
         <v>0.75</v>
       </c>
     </row>
@@ -20729,15 +20736,21 @@
       <c r="C45" s="63">
         <v>20</v>
       </c>
-      <c r="D45" s="63"/>
+      <c r="D45" s="63">
+        <v>6</v>
+      </c>
       <c r="E45" s="64">
-        <v>0</v>
-      </c>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F45" s="65">
+        <v>43899</v>
+      </c>
+      <c r="G45" s="65">
+        <v>43900</v>
+      </c>
+      <c r="H45" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -20758,141 +20771,141 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="67">
-        <v>15</v>
-      </c>
-      <c r="D47" s="67"/>
-      <c r="E47" s="68">
-        <v>0</v>
-      </c>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="193" t="str">
-        <f t="shared" si="11"/>
-        <v/>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="45" t="str">
+      <c r="B49" s="45" t="str">
         <f>B6</f>
         <v>Node.js</v>
       </c>
-      <c r="C50" s="45">
-        <f>SUM(C51:C57)</f>
+      <c r="C49" s="45">
+        <f>SUM(C50:C56)</f>
         <v>80</v>
       </c>
-      <c r="D50" s="45">
-        <f>SUM(D51:D57)</f>
+      <c r="D49" s="45">
+        <f>SUM(D50:D56)</f>
         <v>15</v>
       </c>
-      <c r="E50" s="46">
-        <f>SUM(E51:E57)/COUNTA(B51:B57)</f>
+      <c r="E49" s="46">
+        <f>SUM(E50:E56)/COUNTA(B50:B56)</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="F50" s="47">
-        <f>IF(MIN(F51:F57)=0,"-",MIN(F51:F57))</f>
+      <c r="F49" s="47">
+        <f>IF(MIN(F50:F56)=0,"-",MIN(F50:F56))</f>
         <v>43863</v>
       </c>
-      <c r="G50" s="45" t="str">
-        <f>IF(COUNTBLANK(G51:G57)&lt;&gt;0,"-",MAX(G51:G57))</f>
+      <c r="G49" s="45" t="str">
+        <f>IF(COUNTBLANK(G50:G56)&lt;&gt;0,"-",MAX(G50:G56))</f>
         <v>-</v>
       </c>
-      <c r="H50" s="187">
-        <f>AVERAGE(H51:H57)</f>
+      <c r="H49" s="187">
+        <f>AVERAGE(H50:H56)</f>
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="48" t="str">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="48" t="str">
         <f>'LE COMMENCEMENT'!B8</f>
         <v>HTTP: web por baixo dos panos</v>
       </c>
-      <c r="C51" s="49">
+      <c r="C50" s="49">
         <f>'LE COMMENCEMENT'!C8</f>
         <v>14</v>
       </c>
-      <c r="D51" s="49">
+      <c r="D50" s="49">
         <f>'LE COMMENCEMENT'!D8</f>
         <v>5</v>
       </c>
-      <c r="E51" s="50">
+      <c r="E50" s="50">
         <f>'LE COMMENCEMENT'!E8</f>
         <v>1</v>
       </c>
-      <c r="F51" s="51">
+      <c r="F50" s="51">
         <f>IF('LE COMMENCEMENT'!F8="","",'LE COMMENCEMENT'!F8)</f>
         <v>43863</v>
       </c>
-      <c r="G51" s="51">
+      <c r="G50" s="51">
         <f>IF('LE COMMENCEMENT'!G8="","",'LE COMMENCEMENT'!G8)</f>
         <v>43863</v>
       </c>
-      <c r="H51" s="188">
-        <f t="shared" ref="H51:H57" si="14">IF(G51="","",1-D51/C51)</f>
+      <c r="H50" s="188">
+        <f t="shared" ref="H50:H56" si="14">IF(G50="","",1-D50/C50)</f>
         <v>0.64285714285714279</v>
       </c>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="52" t="str">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="52" t="str">
         <f>B15</f>
         <v>Javascript: prog. na linguagem web</v>
       </c>
-      <c r="C52" s="53">
+      <c r="C51" s="53">
         <f>C15</f>
         <v>20</v>
       </c>
-      <c r="D52" s="53">
+      <c r="D51" s="53">
         <f>D15</f>
         <v>10</v>
       </c>
-      <c r="E52" s="54">
+      <c r="E51" s="54">
         <f>E15</f>
         <v>1</v>
       </c>
-      <c r="F52" s="74">
+      <c r="F51" s="74">
         <f>IF(F15="","",F15)</f>
         <v>43873</v>
       </c>
-      <c r="G52" s="74">
+      <c r="G51" s="74">
         <f>IF(G15="","",G15)</f>
         <v>43877</v>
       </c>
-      <c r="H52" s="189">
+      <c r="H51" s="189">
         <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
     </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="63">
+        <v>12</v>
+      </c>
+      <c r="D52" s="63"/>
+      <c r="E52" s="64">
+        <v>0</v>
+      </c>
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
+      <c r="H52" s="192" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="62" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C53" s="63">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D53" s="63"/>
       <c r="E53" s="64">
@@ -20907,10 +20920,10 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="62" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="C54" s="63">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D54" s="63"/>
       <c r="E54" s="64">
@@ -20925,10 +20938,10 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="62" t="s">
-        <v>161</v>
+        <v>89</v>
       </c>
       <c r="C55" s="63">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D55" s="63"/>
       <c r="E55" s="64">
@@ -20942,112 +20955,112 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="63">
-        <v>6</v>
-      </c>
-      <c r="D56" s="63"/>
-      <c r="E56" s="64">
-        <v>0</v>
-      </c>
-      <c r="F56" s="65"/>
-      <c r="G56" s="65"/>
-      <c r="H56" s="192" t="str">
+      <c r="B56" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="67">
+        <v>4</v>
+      </c>
+      <c r="D56" s="67"/>
+      <c r="E56" s="68">
+        <v>0</v>
+      </c>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="193" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="C57" s="67">
-        <v>4</v>
-      </c>
-      <c r="D57" s="67"/>
-      <c r="E57" s="68">
-        <v>0</v>
-      </c>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="193" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C58" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="45" t="str">
+      <c r="B59" s="45" t="str">
         <f>B7</f>
         <v>React</v>
       </c>
-      <c r="C60" s="45">
-        <f>SUM(C61:C68)</f>
+      <c r="C59" s="45">
+        <f>SUM(C60:C67)</f>
         <v>74</v>
       </c>
-      <c r="D60" s="45">
-        <f>SUM(D61:D68)</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="46">
-        <f>SUM(E61:E68)/COUNTA(B61:B68)</f>
-        <v>0</v>
-      </c>
-      <c r="F60" s="47" t="str">
-        <f>IF(MIN(F61:F68)=0,"-",MIN(F61:F68))</f>
+      <c r="D59" s="45">
+        <f>SUM(D60:D67)</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="46">
+        <f>SUM(E60:E67)/COUNTA(B60:B67)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="47" t="str">
+        <f>IF(MIN(F60:F67)=0,"-",MIN(F60:F67))</f>
         <v>-</v>
       </c>
-      <c r="G60" s="45" t="str">
-        <f>IF(COUNTBLANK(G61:G68)&lt;&gt;0,"-",MAX(G61:G68))</f>
+      <c r="G59" s="45" t="str">
+        <f>IF(COUNTBLANK(G60:G67)&lt;&gt;0,"-",MAX(G60:G67))</f>
         <v>-</v>
       </c>
-      <c r="H60" s="187" t="e">
-        <f>AVERAGE(H61:H68)</f>
+      <c r="H59" s="187" t="e">
+        <f>AVERAGE(H60:H67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="59">
+        <v>12</v>
+      </c>
+      <c r="D60" s="59"/>
+      <c r="E60" s="60">
+        <v>0</v>
+      </c>
+      <c r="F60" s="61"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="191" t="str">
+        <f t="shared" ref="H60:H67" si="15">IF(G60="","",1-D60/C60)</f>
+        <v/>
+      </c>
+    </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="58" t="s">
-        <v>162</v>
-      </c>
-      <c r="C61" s="59">
+      <c r="B61" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" s="63">
         <v>12</v>
       </c>
-      <c r="D61" s="59"/>
-      <c r="E61" s="60">
-        <v>0</v>
-      </c>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="191" t="str">
-        <f t="shared" ref="H61:H68" si="15">IF(G61="","",1-D61/C61)</f>
+      <c r="D61" s="63"/>
+      <c r="E61" s="64">
+        <v>0</v>
+      </c>
+      <c r="F61" s="65"/>
+      <c r="G61" s="65"/>
+      <c r="H61" s="192" t="str">
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="62" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C62" s="63">
         <v>12</v>
@@ -21065,10 +21078,10 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="62" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C63" s="63">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D63" s="63"/>
       <c r="E63" s="64">
@@ -21083,10 +21096,10 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="62" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C64" s="63">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D64" s="63"/>
       <c r="E64" s="64">
@@ -21101,7 +21114,7 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C65" s="63">
         <v>10</v>
@@ -21119,10 +21132,10 @@
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="62" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C66" s="63">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D66" s="63"/>
       <c r="E66" s="64">
@@ -21136,37 +21149,19 @@
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="C67" s="63">
-        <v>8</v>
-      </c>
-      <c r="D67" s="63"/>
-      <c r="E67" s="64">
-        <v>0</v>
-      </c>
-      <c r="F67" s="65"/>
-      <c r="G67" s="65"/>
-      <c r="H67" s="192" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="66" t="s">
+      <c r="B67" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="C68" s="67">
+      <c r="C67" s="67">
         <v>2</v>
       </c>
-      <c r="D68" s="67"/>
-      <c r="E68" s="68">
-        <v>0</v>
-      </c>
-      <c r="F68" s="69"/>
-      <c r="G68" s="69"/>
-      <c r="H68" s="193" t="str">
+      <c r="D67" s="67"/>
+      <c r="E67" s="68">
+        <v>0</v>
+      </c>
+      <c r="F67" s="69"/>
+      <c r="G67" s="69"/>
+      <c r="H67" s="193" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
@@ -21415,11 +21410,11 @@
       </c>
       <c r="D8" s="43">
         <f t="shared" ref="D8:E8" si="0">D79</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E8" s="44">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="F8" s="70">
         <f>IF(F79="-","",F79)</f>
@@ -22758,11 +22753,11 @@
       </c>
       <c r="D79" s="18">
         <f>SUM(D80:D90)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E79" s="19">
         <f>SUM(E80:E90)/COUNTA(B80:B90)</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="F79" s="20">
         <f>IF(MIN(F80:F90)=0,"-",MIN(F80:F90))</f>
@@ -22774,7 +22769,7 @@
       </c>
       <c r="H79" s="199">
         <f>AVERAGE(H80:H90)</f>
-        <v>0.64285714285714279</v>
+        <v>0.67142857142857137</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
@@ -22818,23 +22813,23 @@
       </c>
       <c r="D81" s="39">
         <f>'FRONT-END'!D45</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E81" s="40">
         <f>'FRONT-END'!E45</f>
-        <v>0</v>
-      </c>
-      <c r="F81" s="41" t="str">
+        <v>1</v>
+      </c>
+      <c r="F81" s="41">
         <f>IF('FRONT-END'!F45="","",'FRONT-END'!F45)</f>
-        <v/>
-      </c>
-      <c r="G81" s="41" t="str">
+        <v>43899</v>
+      </c>
+      <c r="G81" s="41">
         <f>IF('FRONT-END'!G45="","",'FRONT-END'!G45)</f>
-        <v/>
-      </c>
-      <c r="H81" s="195" t="str">
+        <v>43900</v>
+      </c>
+      <c r="H81" s="195">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -22869,27 +22864,27 @@
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="38" t="str">
-        <f>'FRONT-END'!B53</f>
+        <f>'FRONT-END'!B52</f>
         <v>Node.js parte 1</v>
       </c>
       <c r="C83" s="39">
-        <f>'FRONT-END'!C53</f>
+        <f>'FRONT-END'!C52</f>
         <v>12</v>
       </c>
       <c r="D83" s="39">
-        <f>'FRONT-END'!D53</f>
+        <f>'FRONT-END'!D52</f>
         <v>0</v>
       </c>
       <c r="E83" s="40">
-        <f>'FRONT-END'!E53</f>
+        <f>'FRONT-END'!E52</f>
         <v>0</v>
       </c>
       <c r="F83" s="41" t="str">
-        <f>IF('FRONT-END'!F53="","",'FRONT-END'!F53)</f>
+        <f>IF('FRONT-END'!F52="","",'FRONT-END'!F52)</f>
         <v/>
       </c>
       <c r="G83" s="41" t="str">
-        <f>IF('FRONT-END'!G53="","",'FRONT-END'!G53)</f>
+        <f>IF('FRONT-END'!G52="","",'FRONT-END'!G52)</f>
         <v/>
       </c>
       <c r="H83" s="195" t="str">
@@ -22899,27 +22894,27 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="38" t="str">
-        <f>'FRONT-END'!B54</f>
+        <f>'FRONT-END'!B53</f>
         <v>Node.js parte 2</v>
       </c>
       <c r="C84" s="39">
-        <f>'FRONT-END'!C54</f>
+        <f>'FRONT-END'!C53</f>
         <v>8</v>
       </c>
       <c r="D84" s="39">
-        <f>'FRONT-END'!D54</f>
+        <f>'FRONT-END'!D53</f>
         <v>0</v>
       </c>
       <c r="E84" s="40">
-        <f>'FRONT-END'!E54</f>
+        <f>'FRONT-END'!E53</f>
         <v>0</v>
       </c>
       <c r="F84" s="41" t="str">
-        <f>IF('FRONT-END'!F54="","",'FRONT-END'!F54)</f>
+        <f>IF('FRONT-END'!F53="","",'FRONT-END'!F53)</f>
         <v/>
       </c>
       <c r="G84" s="41" t="str">
-        <f>IF('FRONT-END'!G54="","",'FRONT-END'!G54)</f>
+        <f>IF('FRONT-END'!G53="","",'FRONT-END'!G53)</f>
         <v/>
       </c>
       <c r="H84" s="195" t="str">
@@ -22983,27 +22978,27 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="38" t="str">
-        <f>'FRONT-END'!B56</f>
+        <f>'FRONT-END'!B55</f>
         <v>MongoDB</v>
       </c>
       <c r="C88" s="39">
-        <f>'FRONT-END'!C56</f>
+        <f>'FRONT-END'!C55</f>
         <v>6</v>
       </c>
       <c r="D88" s="39">
-        <f>'FRONT-END'!D56</f>
+        <f>'FRONT-END'!D55</f>
         <v>0</v>
       </c>
       <c r="E88" s="40">
-        <f>'FRONT-END'!E56</f>
+        <f>'FRONT-END'!E55</f>
         <v>0</v>
       </c>
       <c r="F88" s="41" t="str">
-        <f>IF('FRONT-END'!F56="","",'FRONT-END'!F56)</f>
+        <f>IF('FRONT-END'!F55="","",'FRONT-END'!F55)</f>
         <v/>
       </c>
       <c r="G88" s="41" t="str">
-        <f>IF('FRONT-END'!G56="","",'FRONT-END'!G56)</f>
+        <f>IF('FRONT-END'!G55="","",'FRONT-END'!G55)</f>
         <v/>
       </c>
       <c r="H88" s="195" t="str">

</xml_diff>

<commit_message>
UPD: Enf of course Web Performance part 2 and HTML and CSS formation
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF2AEF5-F86A-485E-81B1-0C2070ED629F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D320323D-AABC-4879-B5F5-F0F23804252E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="284">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3063,8 +3063,8 @@
   </sheetPr>
   <dimension ref="A2:AZ196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT25" sqref="AT25"/>
+    <sheetView tabSelected="1" topLeftCell="U7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT26" sqref="AT26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5127,10 +5127,18 @@
       <c r="AH20" s="166">
         <v>45</v>
       </c>
-      <c r="AI20" s="166"/>
-      <c r="AJ20" s="166"/>
-      <c r="AK20" s="166"/>
-      <c r="AL20" s="169"/>
+      <c r="AI20" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AJ20" s="166">
+        <v>46</v>
+      </c>
+      <c r="AK20" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL20" s="169" t="s">
+        <v>255</v>
+      </c>
       <c r="AP20" s="62" t="s">
         <v>158</v>
       </c>
@@ -5366,7 +5374,9 @@
       <c r="AD22" s="169" t="s">
         <v>255</v>
       </c>
-      <c r="AF22" s="169"/>
+      <c r="AF22" s="183">
+        <v>46</v>
+      </c>
       <c r="AG22" s="166"/>
       <c r="AH22" s="166"/>
       <c r="AI22" s="166"/>
@@ -5752,6 +5762,9 @@
       </c>
       <c r="AS25" s="45" t="s">
         <v>140</v>
+      </c>
+      <c r="AT25" s="180" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -19607,9 +19620,7 @@
   </sheetPr>
   <dimension ref="B2:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19654,11 +19665,11 @@
       </c>
       <c r="D3" s="45">
         <f>SUM(D4:D7)</f>
-        <v>117.5</v>
+        <v>123.5</v>
       </c>
       <c r="E3" s="46">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0.43172268907563027</v>
+        <v>0.4464285714285714</v>
       </c>
       <c r="F3" s="47">
         <f>IF(MIN(F4:F7)=0,"-",MIN(F4:F7))</f>
@@ -19668,9 +19679,9 @@
         <f>IF(COUNTBLANK(G4:G7)&lt;&gt;0,"-",MAX(G4:G7))</f>
         <v>-</v>
       </c>
-      <c r="H3" s="187" t="e">
+      <c r="H3" s="187">
         <f>AVERAGE(H4:H7)</f>
-        <v>#DIV/0!</v>
+        <v>0.56647398843930641</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -19712,23 +19723,23 @@
       </c>
       <c r="D5" s="53">
         <f>D29</f>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E5" s="54">
         <f>E29</f>
-        <v>0.94117647058823528</v>
+        <v>1</v>
       </c>
       <c r="F5" s="53">
         <f>IF(F29="-","",F29)</f>
         <v>43863</v>
       </c>
-      <c r="G5" s="53" t="str">
+      <c r="G5" s="53">
         <f>IF(G29="-","",G29)</f>
-        <v/>
-      </c>
-      <c r="H5" s="189" t="str">
+        <v>43905</v>
+      </c>
+      <c r="H5" s="189">
         <f>IF(G5="","",1-D5/C5)</f>
-        <v/>
+        <v>0.56647398843930641</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -20035,7 +20046,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="53">
-        <f t="shared" si="2"/>
+        <f>D38</f>
         <v>5</v>
       </c>
       <c r="E18" s="54">
@@ -20125,7 +20136,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="53">
-        <f t="shared" si="3"/>
+        <f>D60</f>
         <v>0</v>
       </c>
       <c r="E21" s="54">
@@ -20314,23 +20325,23 @@
       </c>
       <c r="D29" s="45">
         <f>SUM(D30:D46)</f>
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E29" s="46">
         <f>SUM(E30:E46)/COUNTA(B30:B46)</f>
-        <v>0.94117647058823528</v>
+        <v>1</v>
       </c>
       <c r="F29" s="47">
         <f>IF(MIN(F30:F46)=0,"-",MIN(F30:F46))</f>
         <v>43863</v>
       </c>
-      <c r="G29" s="45" t="str">
+      <c r="G29" s="45">
         <f>IF(COUNTBLANK(G30:G46)&lt;&gt;0,"-",MAX(G30:G46))</f>
-        <v>-</v>
+        <v>43905</v>
       </c>
       <c r="H29" s="187">
         <f>AVERAGE(H30:H46)</f>
-        <v>0.50120287698412691</v>
+        <v>0.51289682539682524</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -20760,15 +20771,21 @@
       <c r="C46" s="63">
         <v>20</v>
       </c>
-      <c r="D46" s="63"/>
+      <c r="D46" s="63">
+        <v>6</v>
+      </c>
       <c r="E46" s="64">
-        <v>0</v>
-      </c>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="192" t="str">
+        <v>1</v>
+      </c>
+      <c r="F46" s="65">
+        <v>43902</v>
+      </c>
+      <c r="G46" s="65">
+        <v>43905</v>
+      </c>
+      <c r="H46" s="192">
         <f t="shared" si="11"/>
-        <v/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -21410,11 +21427,11 @@
       </c>
       <c r="D8" s="43">
         <f t="shared" ref="D8:E8" si="0">D79</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E8" s="44">
         <f t="shared" si="0"/>
-        <v>0.18181818181818182</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F8" s="70">
         <f>IF(F79="-","",F79)</f>
@@ -22753,11 +22770,11 @@
       </c>
       <c r="D79" s="18">
         <f>SUM(D80:D90)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E79" s="19">
         <f>SUM(E80:E90)/COUNTA(B80:B90)</f>
-        <v>0.18181818181818182</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F79" s="20">
         <f>IF(MIN(F80:F90)=0,"-",MIN(F80:F90))</f>
@@ -22769,7 +22786,7 @@
       </c>
       <c r="H79" s="199">
         <f>AVERAGE(H80:H90)</f>
-        <v>0.67142857142857137</v>
+        <v>0.68095238095238086</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
@@ -22843,23 +22860,23 @@
       </c>
       <c r="D82" s="39">
         <f>'FRONT-END'!D46</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E82" s="40">
         <f>'FRONT-END'!E46</f>
-        <v>0</v>
-      </c>
-      <c r="F82" s="41" t="str">
+        <v>1</v>
+      </c>
+      <c r="F82" s="41">
         <f>IF('FRONT-END'!F46="","",'FRONT-END'!F46)</f>
-        <v/>
-      </c>
-      <c r="G82" s="41" t="str">
+        <v>43902</v>
+      </c>
+      <c r="G82" s="41">
         <f>IF('FRONT-END'!G46="","",'FRONT-END'!G46)</f>
-        <v/>
-      </c>
-      <c r="H82" s="195" t="str">
+        <v>43905</v>
+      </c>
+      <c r="H82" s="195">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Java part 1
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D320323D-AABC-4879-B5F5-F0F23804252E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4405F56B-369F-4E17-B047-0F42094343C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="284">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3063,8 +3063,8 @@
   </sheetPr>
   <dimension ref="A2:AZ196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT26" sqref="AT26"/>
+    <sheetView tabSelected="1" topLeftCell="N7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI22" sqref="AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5377,8 +5377,12 @@
       <c r="AF22" s="183">
         <v>46</v>
       </c>
-      <c r="AG22" s="166"/>
-      <c r="AH22" s="166"/>
+      <c r="AG22" s="166">
+        <v>13</v>
+      </c>
+      <c r="AH22" s="166">
+        <v>13</v>
+      </c>
       <c r="AI22" s="166"/>
       <c r="AJ22" s="166"/>
       <c r="AK22" s="166"/>
@@ -5861,6 +5865,9 @@
       </c>
       <c r="AS26" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT26" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AZ26" s="178" t="s">
         <v>92</v>
@@ -18686,11 +18693,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D28)</f>
-        <v>50.5</v>
+        <v>53.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E28)/COUNTA(B4:B28)</f>
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F28)=0,"-",MIN(F4:F28))</f>
@@ -18702,7 +18709,7 @@
       </c>
       <c r="H3" s="185">
         <f>AVERAGE(H4:H28)</f>
-        <v>0.58685064935064934</v>
+        <v>0.59002976190476186</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -18994,15 +19001,21 @@
       <c r="C16" s="13">
         <v>8</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="13">
+        <v>3</v>
+      </c>
       <c r="E16" s="14">
-        <v>0</v>
-      </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="184" t="str">
+        <v>1</v>
+      </c>
+      <c r="F16" s="35">
+        <v>43906</v>
+      </c>
+      <c r="G16" s="35">
+        <v>43907</v>
+      </c>
+      <c r="H16" s="184">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.625</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -21282,11 +21295,11 @@
       </c>
       <c r="D3" s="18">
         <f>SUM(D4:D7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" s="19">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>0</v>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="F3" s="20">
         <f>IF(MIN(F4:F8)=0,"-",MIN(F4:F8))</f>
@@ -21311,15 +21324,15 @@
       </c>
       <c r="D4" s="32">
         <f>D11</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="33">
         <f>E11</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="34" t="str">
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="F4" s="34">
         <f>IF(F11="-","",F11)</f>
-        <v/>
+        <v>43906</v>
       </c>
       <c r="G4" s="34" t="str">
         <f>IF(G11="-","",G11)</f>
@@ -21480,23 +21493,23 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(D12:D28)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="19">
         <f>SUM(E12:E28)/COUNTA(B12:B28)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="20" t="str">
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="F11" s="20">
         <f>IF(MIN(F12:F28)=0,"-",MIN(F12:F28))</f>
-        <v>-</v>
+        <v>43906</v>
       </c>
       <c r="G11" s="18" t="str">
         <f>IF(COUNTBLANK(G12:G28)&lt;&gt;0,"-",MAX(G12:G28))</f>
         <v>-</v>
       </c>
-      <c r="H11" s="199" t="e">
+      <c r="H11" s="199">
         <f>AVERAGE(H12:H28)</f>
-        <v>#DIV/0!</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -21510,23 +21523,23 @@
       </c>
       <c r="D12" s="32">
         <f>'LE COMMENCEMENT'!D16</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="33">
         <f>'LE COMMENCEMENT'!E16</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="F12" s="34">
         <f>IF('LE COMMENCEMENT'!F16="","",'LE COMMENCEMENT'!F16)</f>
-        <v/>
-      </c>
-      <c r="G12" s="34" t="str">
+        <v>43906</v>
+      </c>
+      <c r="G12" s="34">
         <f>IF('LE COMMENCEMENT'!G16="","",'LE COMMENCEMENT'!G16)</f>
-        <v/>
-      </c>
-      <c r="H12" s="194" t="str">
+        <v>43907</v>
+      </c>
+      <c r="H12" s="194">
         <f t="shared" ref="H12:H28" si="1">IF(G12="","",1-D12/C12)</f>
-        <v/>
+        <v>0.625</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Java part 2
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4405F56B-369F-4E17-B047-0F42094343C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5D989-DAD9-41F1-B905-EDFC3D9C52EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="284">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3064,7 +3064,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI22" sqref="AI22"/>
+      <selection activeCell="AT28" sqref="AT28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5383,10 +5383,18 @@
       <c r="AH22" s="166">
         <v>13</v>
       </c>
-      <c r="AI22" s="166"/>
-      <c r="AJ22" s="166"/>
-      <c r="AK22" s="166"/>
-      <c r="AL22" s="169"/>
+      <c r="AI22" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AJ22" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK22" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL22" s="169" t="s">
+        <v>255</v>
+      </c>
       <c r="AP22" s="62" t="s">
         <v>159</v>
       </c>
@@ -5613,8 +5621,12 @@
       <c r="AD24" s="169">
         <v>51</v>
       </c>
-      <c r="AF24" s="169"/>
-      <c r="AG24" s="166"/>
+      <c r="AF24" s="169" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG24" s="166">
+        <v>14</v>
+      </c>
       <c r="AH24" s="166"/>
       <c r="AI24" s="166"/>
       <c r="AJ24" s="166"/>
@@ -5999,6 +6011,9 @@
       </c>
       <c r="AS27" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT27" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AZ27" s="1" t="s">
         <v>268</v>
@@ -18644,7 +18659,9 @@
   </sheetPr>
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18693,11 +18710,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D28)</f>
-        <v>53.5</v>
+        <v>56.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E28)/COUNTA(B4:B28)</f>
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F28)=0,"-",MIN(F4:F28))</f>
@@ -18709,7 +18726,7 @@
       </c>
       <c r="H3" s="185">
         <f>AVERAGE(H4:H28)</f>
-        <v>0.59002976190476186</v>
+        <v>0.59271978021978022</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -19025,15 +19042,21 @@
       <c r="C17" s="13">
         <v>8</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13">
+        <v>3</v>
+      </c>
       <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="184" t="str">
+        <v>1</v>
+      </c>
+      <c r="F17" s="35">
+        <v>43913</v>
+      </c>
+      <c r="G17" s="35">
+        <v>43913</v>
+      </c>
+      <c r="H17" s="184">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.625</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -21295,11 +21318,11 @@
       </c>
       <c r="D3" s="18">
         <f>SUM(D4:D7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="19">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>1.4705882352941176E-2</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="F3" s="20">
         <f>IF(MIN(F4:F8)=0,"-",MIN(F4:F8))</f>
@@ -21324,11 +21347,11 @@
       </c>
       <c r="D4" s="32">
         <f>D11</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4" s="33">
         <f>E11</f>
-        <v>5.8823529411764705E-2</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="F4" s="34">
         <f>IF(F11="-","",F11)</f>
@@ -21493,11 +21516,11 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(D12:D28)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" s="19">
         <f>SUM(E12:E28)/COUNTA(B12:B28)</f>
-        <v>5.8823529411764705E-2</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="F11" s="20">
         <f>IF(MIN(F12:F28)=0,"-",MIN(F12:F28))</f>
@@ -21553,23 +21576,23 @@
       </c>
       <c r="D13" s="39">
         <f>'LE COMMENCEMENT'!D17</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" s="40">
         <f>'LE COMMENCEMENT'!E17</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="41" t="str">
+        <v>1</v>
+      </c>
+      <c r="F13" s="41">
         <f>IF('LE COMMENCEMENT'!F17="","",'LE COMMENCEMENT'!F17)</f>
-        <v/>
-      </c>
-      <c r="G13" s="41" t="str">
+        <v>43913</v>
+      </c>
+      <c r="G13" s="41">
         <f>IF('LE COMMENCEMENT'!G17="","",'LE COMMENCEMENT'!G17)</f>
-        <v/>
-      </c>
-      <c r="H13" s="195" t="str">
+        <v>43913</v>
+      </c>
+      <c r="H13" s="195">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.625</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Java part 3
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5D989-DAD9-41F1-B905-EDFC3D9C52EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A764A-B174-4AA8-8279-7BF925B6DF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="284">
   <si>
     <t>Le commencement</t>
   </si>
@@ -2501,7 +2501,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -3064,7 +3064,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT28" sqref="AT28"/>
+      <selection activeCell="AT29" sqref="AT29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5627,7 +5627,9 @@
       <c r="AG24" s="166">
         <v>14</v>
       </c>
-      <c r="AH24" s="166"/>
+      <c r="AH24" s="166">
+        <v>15</v>
+      </c>
       <c r="AI24" s="166"/>
       <c r="AJ24" s="166"/>
       <c r="AK24" s="166"/>
@@ -6113,6 +6115,9 @@
       </c>
       <c r="AS28" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT28" s="180" t="s">
+        <v>277</v>
       </c>
       <c r="AZ28" s="179" t="s">
         <v>269</v>
@@ -18660,7 +18665,7 @@
   <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -18710,11 +18715,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D28)</f>
-        <v>56.5</v>
+        <v>66.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E28)/COUNTA(B4:B28)</f>
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F28)=0,"-",MIN(F4:F28))</f>
@@ -18726,7 +18731,7 @@
       </c>
       <c r="H3" s="185">
         <f>AVERAGE(H4:H28)</f>
-        <v>0.59271978021978022</v>
+        <v>0.57716836734693877</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -19066,15 +19071,21 @@
       <c r="C18" s="13">
         <v>16</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13">
+        <v>10</v>
+      </c>
       <c r="E18" s="14">
-        <v>0</v>
-      </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="184" t="str">
+        <v>1</v>
+      </c>
+      <c r="F18" s="35">
+        <v>43914</v>
+      </c>
+      <c r="G18" s="35">
+        <v>43916</v>
+      </c>
+      <c r="H18" s="184">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -21318,11 +21329,11 @@
       </c>
       <c r="D3" s="18">
         <f>SUM(D4:D7)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E3" s="19">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>2.9411764705882353E-2</v>
+        <v>4.4117647058823532E-2</v>
       </c>
       <c r="F3" s="20">
         <f>IF(MIN(F4:F8)=0,"-",MIN(F4:F8))</f>
@@ -21347,11 +21358,11 @@
       </c>
       <c r="D4" s="32">
         <f>D11</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E4" s="33">
         <f>E11</f>
-        <v>0.11764705882352941</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="F4" s="34">
         <f>IF(F11="-","",F11)</f>
@@ -21516,11 +21527,11 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(D12:D28)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E11" s="19">
         <f>SUM(E12:E28)/COUNTA(B12:B28)</f>
-        <v>0.11764705882352941</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="F11" s="20">
         <f>IF(MIN(F12:F28)=0,"-",MIN(F12:F28))</f>
@@ -21532,7 +21543,7 @@
       </c>
       <c r="H11" s="199">
         <f>AVERAGE(H12:H28)</f>
-        <v>0.625</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -21606,23 +21617,23 @@
       </c>
       <c r="D14" s="39">
         <f>'LE COMMENCEMENT'!D18</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E14" s="40">
         <f>'LE COMMENCEMENT'!E18</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="41" t="str">
+        <v>1</v>
+      </c>
+      <c r="F14" s="41">
         <f>IF('LE COMMENCEMENT'!F18="","",'LE COMMENCEMENT'!F18)</f>
-        <v/>
-      </c>
-      <c r="G14" s="41" t="str">
+        <v>43914</v>
+      </c>
+      <c r="G14" s="41">
         <f>IF('LE COMMENCEMENT'!G18="","",'LE COMMENCEMENT'!G18)</f>
-        <v/>
-      </c>
-      <c r="H14" s="195" t="str">
+        <v>43916</v>
+      </c>
+      <c r="H14" s="195">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Java part 4
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A764A-B174-4AA8-8279-7BF925B6DF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D577C2E9-7A8B-461E-93B8-F29411FC02E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="284">
   <si>
     <t>Le commencement</t>
   </si>
@@ -3064,7 +3064,7 @@
   <dimension ref="A2:AZ196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT29" sqref="AT29"/>
+      <selection activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5630,10 +5630,18 @@
       <c r="AH24" s="166">
         <v>15</v>
       </c>
-      <c r="AI24" s="166"/>
-      <c r="AJ24" s="166"/>
-      <c r="AK24" s="166"/>
-      <c r="AL24" s="169"/>
+      <c r="AI24" s="166">
+        <v>15</v>
+      </c>
+      <c r="AJ24" s="166">
+        <v>15</v>
+      </c>
+      <c r="AK24" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL24" s="169" t="s">
+        <v>255</v>
+      </c>
       <c r="AP24" s="62" t="s">
         <v>82</v>
       </c>
@@ -5860,9 +5868,15 @@
       <c r="AD26" s="169">
         <v>54</v>
       </c>
-      <c r="AF26" s="169"/>
-      <c r="AG26" s="166"/>
-      <c r="AH26" s="166"/>
+      <c r="AF26" s="169" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG26" s="166" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH26" s="166">
+        <v>16</v>
+      </c>
       <c r="AI26" s="166"/>
       <c r="AJ26" s="166"/>
       <c r="AK26" s="166"/>
@@ -6249,6 +6263,9 @@
       </c>
       <c r="AS29" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="AT29" s="180" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18665,7 +18682,7 @@
   <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -18715,11 +18732,11 @@
       </c>
       <c r="D3" s="4">
         <f>SUM(D4:D28)</f>
-        <v>66.5</v>
+        <v>70.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(E4:E28)/COUNTA(B4:B28)</f>
-        <v>0.56000000000000005</v>
+        <v>0.6</v>
       </c>
       <c r="F3" s="5">
         <f>IF(MIN(F4:F28)=0,"-",MIN(F4:F28))</f>
@@ -18731,7 +18748,7 @@
       </c>
       <c r="H3" s="185">
         <f>AVERAGE(H4:H28)</f>
-        <v>0.57716836734693877</v>
+        <v>0.58313492063492056</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -19095,15 +19112,21 @@
       <c r="C19" s="13">
         <v>12</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="13">
+        <v>4</v>
+      </c>
       <c r="E19" s="14">
-        <v>0</v>
-      </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="184" t="str">
+        <v>1</v>
+      </c>
+      <c r="F19" s="35">
+        <v>43921</v>
+      </c>
+      <c r="G19" s="35">
+        <v>43921</v>
+      </c>
+      <c r="H19" s="184">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -21280,7 +21303,9 @@
   </sheetPr>
   <dimension ref="B1:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21329,11 +21354,11 @@
       </c>
       <c r="D3" s="18">
         <f>SUM(D4:D7)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E3" s="19">
         <f>SUM(E4:E7)/COUNTA(B4:B7)</f>
-        <v>4.4117647058823532E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="F3" s="20">
         <f>IF(MIN(F4:F8)=0,"-",MIN(F4:F8))</f>
@@ -21358,11 +21383,11 @@
       </c>
       <c r="D4" s="32">
         <f>D11</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E4" s="33">
         <f>E11</f>
-        <v>0.17647058823529413</v>
+        <v>0.23529411764705882</v>
       </c>
       <c r="F4" s="34">
         <f>IF(F11="-","",F11)</f>
@@ -21527,11 +21552,11 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(D12:D28)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E11" s="19">
         <f>SUM(E12:E28)/COUNTA(B12:B28)</f>
-        <v>0.17647058823529413</v>
+        <v>0.23529411764705882</v>
       </c>
       <c r="F11" s="20">
         <f>IF(MIN(F12:F28)=0,"-",MIN(F12:F28))</f>
@@ -21543,7 +21568,7 @@
       </c>
       <c r="H11" s="199">
         <f>AVERAGE(H12:H28)</f>
-        <v>0.54166666666666663</v>
+        <v>0.57291666666666674</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -21647,23 +21672,23 @@
       </c>
       <c r="D15" s="39">
         <f>'LE COMMENCEMENT'!D19</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15" s="40">
         <f>'LE COMMENCEMENT'!E19</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="41" t="str">
+        <v>1</v>
+      </c>
+      <c r="F15" s="41">
         <f>IF('LE COMMENCEMENT'!F19="","",'LE COMMENCEMENT'!F19)</f>
-        <v/>
-      </c>
-      <c r="G15" s="41" t="str">
+        <v>43921</v>
+      </c>
+      <c r="G15" s="41">
         <f>IF('LE COMMENCEMENT'!G19="","",'LE COMMENCEMENT'!G19)</f>
-        <v/>
-      </c>
-      <c r="H15" s="195" t="str">
+        <v>43921</v>
+      </c>
+      <c r="H15" s="195">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UPD: End of course Python for Data Science: Pandas
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB8741-7AD4-4D68-A8BE-CDCC0A02D587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB10C8AC-26E2-438E-AD51-AC9764E7336F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="267">
   <si>
     <t>Le commencement</t>
   </si>
@@ -2458,8 +2452,8 @@
   </sheetPr>
   <dimension ref="A2:AZ208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG32" sqref="AG32"/>
+    <sheetView tabSelected="1" topLeftCell="O16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AP42" sqref="AP42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6079,9 +6073,15 @@
       <c r="AF32" s="76">
         <v>139</v>
       </c>
-      <c r="AG32" s="73"/>
-      <c r="AH32" s="73"/>
-      <c r="AI32" s="73"/>
+      <c r="AG32" s="73" t="s">
+        <v>231</v>
+      </c>
+      <c r="AH32" s="73">
+        <v>30</v>
+      </c>
+      <c r="AI32" s="73">
+        <v>31</v>
+      </c>
       <c r="AJ32" s="73"/>
       <c r="AK32" s="73"/>
       <c r="AL32" s="76"/>
@@ -7055,7 +7055,7 @@
       </c>
       <c r="AT40" s="87" t="str">
         <f t="shared" si="153"/>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="41" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -7192,7 +7192,7 @@
       </c>
       <c r="AT41" s="87" t="str">
         <f t="shared" si="153"/>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="42" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UPD: End of course Statistics part 1
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB10C8AC-26E2-438E-AD51-AC9764E7336F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF506E44-089E-4466-B924-21BC0E084DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="267">
   <si>
     <t>Le commencement</t>
   </si>
@@ -2453,7 +2453,7 @@
   <dimension ref="A2:AZ208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AP42" sqref="AP42"/>
+      <selection activeCell="AT43" sqref="AT43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6082,9 +6082,15 @@
       <c r="AI32" s="73">
         <v>31</v>
       </c>
-      <c r="AJ32" s="73"/>
-      <c r="AK32" s="73"/>
-      <c r="AL32" s="76"/>
+      <c r="AJ32" s="73">
+        <v>32</v>
+      </c>
+      <c r="AK32" s="73" t="s">
+        <v>231</v>
+      </c>
+      <c r="AL32" s="76" t="s">
+        <v>231</v>
+      </c>
       <c r="AP32" s="12" t="s">
         <v>261</v>
       </c>
@@ -6317,9 +6323,15 @@
       <c r="AD34" s="76">
         <v>33</v>
       </c>
-      <c r="AF34" s="76"/>
-      <c r="AG34" s="73"/>
-      <c r="AH34" s="73"/>
+      <c r="AF34" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="AG34" s="73">
+        <v>32</v>
+      </c>
+      <c r="AH34" s="73">
+        <v>32</v>
+      </c>
       <c r="AI34" s="73"/>
       <c r="AJ34" s="73"/>
       <c r="AK34" s="73"/>
@@ -7294,7 +7306,7 @@
       </c>
       <c r="AT42" s="87" t="str">
         <f t="shared" si="153"/>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="43" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UPD: End of course Statistics part 2
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF506E44-089E-4466-B924-21BC0E084DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3D77A1-EE27-40E4-A170-8AE5B384DBD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -2453,7 +2453,7 @@
   <dimension ref="A2:AZ208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT43" sqref="AT43"/>
+      <selection activeCell="AJ34" sqref="AJ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6332,7 +6332,9 @@
       <c r="AH34" s="73">
         <v>32</v>
       </c>
-      <c r="AI34" s="73"/>
+      <c r="AI34" s="73">
+        <v>33</v>
+      </c>
       <c r="AJ34" s="73"/>
       <c r="AK34" s="73"/>
       <c r="AL34" s="76"/>
@@ -7440,7 +7442,7 @@
       </c>
       <c r="AT43" s="87" t="str">
         <f t="shared" si="153"/>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="44" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UPD: End of course Introduction to SQL using MySQL
</commit_message>
<xml_diff>
--- a/Planejamento.xlsx
+++ b/Planejamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela Gandorphi\Documents\Estudos\Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5FDD20-BE26-4E21-B4C3-57C0E854744B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6BE99F-562F-4432-B224-4E6E1057D576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="724" xr2:uid="{2ADBD83B-F3FB-4BB6-B18E-95839D6004A8}"/>
   </bookViews>
@@ -1914,14 +1914,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1929,6 +1922,37 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2006,25 +2030,11 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2452,8 +2462,8 @@
   </sheetPr>
   <dimension ref="A2:AZ208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X44" sqref="X44"/>
+    <sheetView tabSelected="1" topLeftCell="P15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG36" sqref="AG36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2701,7 +2711,7 @@
         <v>10</v>
       </c>
       <c r="AR5" s="56">
-        <f t="shared" ref="AR5:AR68" si="3">INDEX(F:F,MATCH(AP5,D:D,0))</f>
+        <f t="shared" ref="AR5:AR45" si="3">INDEX(F:F,MATCH(AP5,D:D,0))</f>
         <v>2</v>
       </c>
       <c r="AS5" s="3" t="str">
@@ -6576,7 +6586,9 @@
       <c r="AD36" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="AF36" s="76"/>
+      <c r="AF36" s="76">
+        <v>12</v>
+      </c>
       <c r="AG36" s="73"/>
       <c r="AH36" s="73"/>
       <c r="AI36" s="73"/>
@@ -7764,7 +7776,7 @@
       </c>
       <c r="AT46" s="87" t="str">
         <f t="shared" ref="AT46:AT109" si="274">IF(COUNTIF(AF:AL,AR46)&lt;&gt;0,"OK","")</f>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="47" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -17393,98 +17405,103 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="containsText" dxfId="18" priority="57" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="19" priority="58" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6:AD70 AF6:AL70">
-    <cfRule type="containsText" dxfId="17" priority="56" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="18" priority="57" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",X6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="16" priority="55">
+    <cfRule type="expression" dxfId="17" priority="56">
       <formula>COUNTIF($X:$AD,$F1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:K1048576">
-    <cfRule type="expression" dxfId="15" priority="54">
+    <cfRule type="expression" dxfId="16" priority="55">
       <formula>COUNTIF($X:$AD,H1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y71">
-    <cfRule type="containsText" dxfId="14" priority="53" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="15" priority="54" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Y71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y72:AD72">
-    <cfRule type="containsText" dxfId="13" priority="52" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="14" priority="53" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Y72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z71:AD71">
-    <cfRule type="containsText" dxfId="12" priority="51" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="13" priority="52" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Z71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X73:AD73">
-    <cfRule type="containsText" dxfId="11" priority="50" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="12" priority="51" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",X73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X75:AB75 Y76:AB76">
-    <cfRule type="containsText" dxfId="10" priority="49" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="11" priority="50" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",X75)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AT1:AT45 AT147:AT1048576 AT54:AT138">
-    <cfRule type="containsText" dxfId="1" priority="19" operator="containsText" text="ok">
+  <conditionalFormatting sqref="AT1:AT45 AT147:AT1048576">
+    <cfRule type="containsText" dxfId="10" priority="20" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",AT1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG71">
-    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",AG71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG72:AL72">
-    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="8" priority="17" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",AG72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH71:AL71">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",AH71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF73:AL74">
-    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",AF73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF75:AJ75 AG76:AJ76">
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="5" priority="14" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",AF75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF76">
-    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",AF76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR210 AR148:AR208 AR228:AR1048576 AR1:AR138">
-    <cfRule type="expression" dxfId="0" priority="58">
+    <cfRule type="expression" dxfId="3" priority="59">
       <formula>COUNTIF($X:$AD,$AR1)&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X74:AD74">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",X74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X76">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",X76)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT46:AT138">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",AT46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>